<commit_message>
Added Spine SABR templates
</commit_message>
<xml_diff>
--- a/External Beam Templates/Structure Templates/Template Spreadsheets/Chest and Abdomen Templates.xlsx
+++ b/External Beam Templates/Structure Templates/Template Spreadsheets/Chest and Abdomen Templates.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\dkphysicspv1\e$\Gregs_Work\Eclipse\Template Management\External Beam Templates\Structure Templates\Template Spreadsheets\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="14385" yWindow="-15" windowWidth="14430" windowHeight="12165" tabRatio="837"/>
+    <workbookView xWindow="14385" yWindow="-15" windowWidth="14430" windowHeight="12165" tabRatio="837" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Abdomen Anatomy" sheetId="2" r:id="rId1"/>
@@ -14,16 +19,18 @@
     <sheet name="Lung VMAT" sheetId="5" r:id="rId5"/>
     <sheet name="Lung SBRT" sheetId="6" r:id="rId6"/>
     <sheet name="Breast" sheetId="7" r:id="rId7"/>
+    <sheet name="Spine" sheetId="8" r:id="rId8"/>
+    <sheet name="Spine OAR" sheetId="9" r:id="rId9"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId8"/>
+    <externalReference r:id="rId10"/>
   </externalReferences>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="853" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1055" uniqueCount="276">
   <si>
     <t>Ribs</t>
   </si>
@@ -779,13 +786,85 @@
   </si>
   <si>
     <t>Planning Target Volume Low</t>
+  </si>
+  <si>
+    <t>PTV for optimizer</t>
+  </si>
+  <si>
+    <t>PRV2 SpinalCanal</t>
+  </si>
+  <si>
+    <t>SpinalCanal PRV 2mm</t>
+  </si>
+  <si>
+    <t>Brain Stem</t>
+  </si>
+  <si>
+    <t>BrainStem</t>
+  </si>
+  <si>
+    <t>Brain Stem PRV</t>
+  </si>
+  <si>
+    <t>PRV2 BrainStem</t>
+  </si>
+  <si>
+    <t>Brain Stem PRV 2mm</t>
+  </si>
+  <si>
+    <t>Spinal Cord</t>
+  </si>
+  <si>
+    <t>PRV2 SpinalCord</t>
+  </si>
+  <si>
+    <t>Spine</t>
+  </si>
+  <si>
+    <t>Spine SBRT</t>
+  </si>
+  <si>
+    <t>.Spine</t>
+  </si>
+  <si>
+    <t>Spine Template.xml</t>
+  </si>
+  <si>
+    <t>Spine OAR</t>
+  </si>
+  <si>
+    <t>OAR for Spine SABR</t>
+  </si>
+  <si>
+    <t>Spine OARTemplate.xml</t>
+  </si>
+  <si>
+    <t>Avoid</t>
+  </si>
+  <si>
+    <t>Avoid Post</t>
+  </si>
+  <si>
+    <t>Post Avoidance Structure</t>
+  </si>
+  <si>
+    <t>Small intestine</t>
+  </si>
+  <si>
+    <t>Large intestine</t>
+  </si>
+  <si>
+    <t>Sacral plexus</t>
+  </si>
+  <si>
+    <t>Urethra</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -824,6 +903,12 @@
       <name val="Cambria"/>
       <family val="2"/>
       <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1153,7 +1238,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1318,12 +1403,571 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Title 2" xfId="1"/>
   </cellStyles>
-  <dxfs count="90">
+  <dxfs count="118">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -2961,63 +3605,109 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table331323431" displayName="Table331323431" ref="A2:B13" totalsRowShown="0" headerRowDxfId="89" headerRowBorderDxfId="88" tableBorderDxfId="87" totalsRowBorderDxfId="86">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table331323431" displayName="Table331323431" ref="A2:B13" totalsRowShown="0" headerRowDxfId="117" headerRowBorderDxfId="116" tableBorderDxfId="115" totalsRowBorderDxfId="114">
   <tableColumns count="2">
     <tableColumn id="1" name="Attribute"/>
-    <tableColumn id="2" name="Value" dataDxfId="85"/>
+    <tableColumn id="2" name="Value" dataDxfId="113"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table5333539" displayName="Table5333539" ref="D2:H38" totalsRowShown="0" headerRowDxfId="35" headerRowBorderDxfId="34" tableBorderDxfId="33" totalsRowBorderDxfId="32">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table5333539" displayName="Table5333539" ref="D2:H38" totalsRowShown="0" headerRowDxfId="63" headerRowBorderDxfId="62" tableBorderDxfId="61" totalsRowBorderDxfId="60">
   <tableColumns count="5">
-    <tableColumn id="1" name="Structure" dataDxfId="31"/>
-    <tableColumn id="2" name="ID" dataDxfId="30"/>
-    <tableColumn id="3" name="Name" dataDxfId="29"/>
-    <tableColumn id="4" name="VolumeCode" dataDxfId="28"/>
-    <tableColumn id="5" name="VolumeCodeTable" dataDxfId="27"/>
+    <tableColumn id="1" name="Structure" dataDxfId="59"/>
+    <tableColumn id="2" name="ID" dataDxfId="58"/>
+    <tableColumn id="3" name="Name" dataDxfId="57"/>
+    <tableColumn id="4" name="VolumeCode" dataDxfId="56"/>
+    <tableColumn id="5" name="VolumeCodeTable" dataDxfId="55"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table3313234" displayName="Table3313234" ref="A2:B13" totalsRowShown="0" headerRowDxfId="26" headerRowBorderDxfId="25" tableBorderDxfId="24" totalsRowBorderDxfId="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table3313234" displayName="Table3313234" ref="A2:B13" totalsRowShown="0" headerRowDxfId="54" headerRowBorderDxfId="53" tableBorderDxfId="52" totalsRowBorderDxfId="51">
   <tableColumns count="2">
     <tableColumn id="1" name="Attribute"/>
-    <tableColumn id="2" name="Value" dataDxfId="22"/>
+    <tableColumn id="2" name="Value" dataDxfId="50"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Table53335" displayName="Table53335" ref="D2:H47" totalsRowShown="0" headerRowDxfId="21" headerRowBorderDxfId="20" tableBorderDxfId="19" totalsRowBorderDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Table53335" displayName="Table53335" ref="D2:H47" totalsRowShown="0" headerRowDxfId="49" headerRowBorderDxfId="48" tableBorderDxfId="47" totalsRowBorderDxfId="46">
   <tableColumns count="5">
-    <tableColumn id="1" name="Structure" dataDxfId="17"/>
-    <tableColumn id="2" name="ID" dataDxfId="16"/>
-    <tableColumn id="3" name="Name" dataDxfId="15"/>
-    <tableColumn id="4" name="VolumeCode" dataDxfId="14"/>
-    <tableColumn id="5" name="VolumeCodeTable" dataDxfId="13"/>
+    <tableColumn id="1" name="Structure" dataDxfId="45"/>
+    <tableColumn id="2" name="ID" dataDxfId="44"/>
+    <tableColumn id="3" name="Name" dataDxfId="43"/>
+    <tableColumn id="4" name="VolumeCode" dataDxfId="42"/>
+    <tableColumn id="5" name="VolumeCodeTable" dataDxfId="41"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Table33132343865" displayName="Table33132343865" ref="A2:B13" totalsRowShown="0" headerRowDxfId="12" headerRowBorderDxfId="11" tableBorderDxfId="10" totalsRowBorderDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Table33132343865" displayName="Table33132343865" ref="A2:B13" totalsRowShown="0" headerRowDxfId="40" headerRowBorderDxfId="39" tableBorderDxfId="38" totalsRowBorderDxfId="37">
   <tableColumns count="2">
     <tableColumn id="1" name="Attribute"/>
-    <tableColumn id="2" name="Value" dataDxfId="8"/>
+    <tableColumn id="2" name="Value" dataDxfId="36"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="Table533353966" displayName="Table533353966" ref="D2:H34" totalsRowShown="0" headerRowBorderDxfId="7" tableBorderDxfId="6" totalsRowBorderDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="Table533353966" displayName="Table533353966" ref="D2:H34" totalsRowShown="0" headerRowBorderDxfId="35" tableBorderDxfId="34" totalsRowBorderDxfId="33">
+  <tableColumns count="5">
+    <tableColumn id="1" name="Structure" dataDxfId="32"/>
+    <tableColumn id="2" name="ID" dataDxfId="31"/>
+    <tableColumn id="3" name="Name" dataDxfId="30"/>
+    <tableColumn id="4" name="VolumeCode" dataDxfId="29"/>
+    <tableColumn id="5" name="VolumeCodeTable" dataDxfId="28"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="15" name="Table3313234386716" displayName="Table3313234386716" ref="A2:B13" totalsRowShown="0" headerRowDxfId="27" headerRowBorderDxfId="25" tableBorderDxfId="26" totalsRowBorderDxfId="24">
+  <tableColumns count="2">
+    <tableColumn id="1" name="Attribute"/>
+    <tableColumn id="2" name="Value" dataDxfId="23"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16" name="Table53335396817" displayName="Table53335396817" ref="D2:H20" totalsRowShown="0" headerRowDxfId="22" headerRowBorderDxfId="20" tableBorderDxfId="21" totalsRowBorderDxfId="19">
+  <tableColumns count="5">
+    <tableColumn id="1" name="Structure" dataDxfId="18"/>
+    <tableColumn id="2" name="ID" dataDxfId="17"/>
+    <tableColumn id="3" name="Name" dataDxfId="16"/>
+    <tableColumn id="4" name="VolumeCode" dataDxfId="15"/>
+    <tableColumn id="5" name="VolumeCodeTable" dataDxfId="14"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="Table331323438671618" displayName="Table331323438671618" ref="A2:B13" totalsRowShown="0" headerRowDxfId="13" headerRowBorderDxfId="11" tableBorderDxfId="12" totalsRowBorderDxfId="10">
+  <tableColumns count="2">
+    <tableColumn id="1" name="Attribute"/>
+    <tableColumn id="2" name="Value" dataDxfId="9"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="Table5333539681719" displayName="Table5333539681719" ref="D2:H25" totalsRowShown="0" headerRowDxfId="8" headerRowBorderDxfId="6" tableBorderDxfId="7" totalsRowBorderDxfId="5">
   <tableColumns count="5">
     <tableColumn id="1" name="Structure" dataDxfId="4"/>
     <tableColumn id="2" name="ID" dataDxfId="3"/>
@@ -3030,86 +3720,86 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table5333537" displayName="Table5333537" ref="D2:F23" totalsRowShown="0" headerRowDxfId="84" headerRowBorderDxfId="83" tableBorderDxfId="82" totalsRowBorderDxfId="81">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table5333537" displayName="Table5333537" ref="D2:F23" totalsRowShown="0" headerRowDxfId="112" headerRowBorderDxfId="111" tableBorderDxfId="110" totalsRowBorderDxfId="109">
   <tableColumns count="3">
-    <tableColumn id="1" name="Structure" dataDxfId="80"/>
-    <tableColumn id="2" name="ID" dataDxfId="79"/>
-    <tableColumn id="3" name="Name" dataDxfId="78"/>
+    <tableColumn id="1" name="Structure" dataDxfId="108"/>
+    <tableColumn id="2" name="ID" dataDxfId="107"/>
+    <tableColumn id="3" name="Name" dataDxfId="106"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table33132343157" displayName="Table33132343157" ref="A2:B13" totalsRowShown="0" headerRowDxfId="77" headerRowBorderDxfId="76" tableBorderDxfId="75" totalsRowBorderDxfId="74">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table33132343157" displayName="Table33132343157" ref="A2:B13" totalsRowShown="0" headerRowDxfId="105" headerRowBorderDxfId="104" tableBorderDxfId="103" totalsRowBorderDxfId="102">
   <tableColumns count="2">
     <tableColumn id="1" name="Attribute"/>
-    <tableColumn id="2" name="Value" dataDxfId="73"/>
+    <tableColumn id="2" name="Value" dataDxfId="101"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table533353758" displayName="Table533353758" ref="D2:F12" totalsRowShown="0" headerRowBorderDxfId="72" tableBorderDxfId="71" totalsRowBorderDxfId="70">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table533353758" displayName="Table533353758" ref="D2:F12" totalsRowShown="0" headerRowBorderDxfId="100" tableBorderDxfId="99" totalsRowBorderDxfId="98">
   <tableColumns count="3">
-    <tableColumn id="1" name="Structure" dataDxfId="69"/>
-    <tableColumn id="2" name="ID" dataDxfId="68"/>
-    <tableColumn id="3" name="Name" dataDxfId="67"/>
+    <tableColumn id="1" name="Structure" dataDxfId="97"/>
+    <tableColumn id="2" name="ID" dataDxfId="96"/>
+    <tableColumn id="3" name="Name" dataDxfId="95"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table35132127" displayName="Table35132127" ref="A2:B13" totalsRowShown="0" headerRowDxfId="66" headerRowBorderDxfId="65" tableBorderDxfId="64" totalsRowBorderDxfId="63">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table35132127" displayName="Table35132127" ref="A2:B13" totalsRowShown="0" headerRowDxfId="94" headerRowBorderDxfId="93" tableBorderDxfId="92" totalsRowBorderDxfId="91">
   <tableColumns count="2">
     <tableColumn id="1" name="Attribute"/>
-    <tableColumn id="2" name="Value" dataDxfId="62"/>
+    <tableColumn id="2" name="Value" dataDxfId="90"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table5142630" displayName="Table5142630" ref="D2:F16" totalsRowShown="0" headerRowDxfId="61" headerRowBorderDxfId="60" tableBorderDxfId="59" totalsRowBorderDxfId="58">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table5142630" displayName="Table5142630" ref="D2:F16" totalsRowShown="0" headerRowDxfId="89" headerRowBorderDxfId="88" tableBorderDxfId="87" totalsRowBorderDxfId="86">
   <tableColumns count="3">
-    <tableColumn id="1" name="Structure" dataDxfId="57"/>
-    <tableColumn id="2" name="ID" dataDxfId="56"/>
-    <tableColumn id="3" name="Name" dataDxfId="55"/>
+    <tableColumn id="1" name="Structure" dataDxfId="85"/>
+    <tableColumn id="2" name="ID" dataDxfId="84"/>
+    <tableColumn id="3" name="Name" dataDxfId="83"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table33132343867" displayName="Table33132343867" ref="A2:B13" totalsRowShown="0" headerRowDxfId="54" headerRowBorderDxfId="53" tableBorderDxfId="52" totalsRowBorderDxfId="51">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table33132343867" displayName="Table33132343867" ref="A2:B13" totalsRowShown="0" headerRowDxfId="82" headerRowBorderDxfId="81" tableBorderDxfId="80" totalsRowBorderDxfId="79">
   <tableColumns count="2">
     <tableColumn id="1" name="Attribute"/>
-    <tableColumn id="2" name="Value" dataDxfId="50"/>
+    <tableColumn id="2" name="Value" dataDxfId="78"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table533353968" displayName="Table533353968" ref="D2:H21" totalsRowShown="0" headerRowDxfId="49" headerRowBorderDxfId="48" tableBorderDxfId="47" totalsRowBorderDxfId="46">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table533353968" displayName="Table533353968" ref="D2:H21" totalsRowShown="0" headerRowDxfId="77" headerRowBorderDxfId="76" tableBorderDxfId="75" totalsRowBorderDxfId="74">
   <tableColumns count="5">
-    <tableColumn id="1" name="Structure" dataDxfId="45"/>
-    <tableColumn id="2" name="ID" dataDxfId="44"/>
-    <tableColumn id="3" name="Name" dataDxfId="43"/>
-    <tableColumn id="4" name="VolumeCode" dataDxfId="42"/>
-    <tableColumn id="5" name="VolumeCodeTable" dataDxfId="41"/>
+    <tableColumn id="1" name="Structure" dataDxfId="73"/>
+    <tableColumn id="2" name="ID" dataDxfId="72"/>
+    <tableColumn id="3" name="Name" dataDxfId="71"/>
+    <tableColumn id="4" name="VolumeCode" dataDxfId="70"/>
+    <tableColumn id="5" name="VolumeCodeTable" dataDxfId="69"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table331323438" displayName="Table331323438" ref="A2:B13" totalsRowShown="0" headerRowDxfId="40" headerRowBorderDxfId="39" tableBorderDxfId="38" totalsRowBorderDxfId="37">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table331323438" displayName="Table331323438" ref="A2:B13" totalsRowShown="0" headerRowDxfId="68" headerRowBorderDxfId="67" tableBorderDxfId="66" totalsRowBorderDxfId="65">
   <tableColumns count="2">
     <tableColumn id="1" name="Attribute"/>
-    <tableColumn id="2" name="Value" dataDxfId="36"/>
+    <tableColumn id="2" name="Value" dataDxfId="64"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3158,7 +3848,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3193,7 +3883,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3407,8 +4097,8 @@
   </sheetPr>
   <dimension ref="A1:S23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5658,7 +6348,7 @@
   <dimension ref="A1:S16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D10" sqref="D10:F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10520,8 +11210,8 @@
   </sheetPr>
   <dimension ref="A1:U53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37:F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15606,4 +16296,2762 @@
     <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:U25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13:H13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.5703125" style="59" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.42578125" style="59" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.42578125" style="59" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" style="59" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" style="59" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.42578125" style="59" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" style="59" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.85546875" style="59" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.85546875" style="59" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="15.42578125" style="59" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.7109375" style="59" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21" style="59" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.7109375" style="59" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.42578125" style="59" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.28515625" style="59" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.42578125" style="59" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.140625" style="59" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.42578125" style="59" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14" style="59" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.42578125" style="59" bestFit="1" customWidth="1"/>
+    <col min="22" max="16384" width="9.140625" style="59"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="62" t="s">
+        <v>262</v>
+      </c>
+      <c r="B1" s="62"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="62" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="62"/>
+      <c r="H1" s="62"/>
+      <c r="J1" s="60" t="s">
+        <v>54</v>
+      </c>
+      <c r="K1" s="63"/>
+      <c r="L1" s="63"/>
+      <c r="M1" s="61"/>
+      <c r="N1" s="60" t="s">
+        <v>53</v>
+      </c>
+      <c r="O1" s="63"/>
+      <c r="P1" s="51" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q1" s="60" t="s">
+        <v>51</v>
+      </c>
+      <c r="R1" s="63"/>
+      <c r="S1" s="61"/>
+      <c r="T1" s="60" t="s">
+        <v>50</v>
+      </c>
+      <c r="U1" s="61"/>
+    </row>
+    <row r="2" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="42" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" s="50" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="24"/>
+      <c r="D2" s="42" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="41" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" s="40" t="s">
+        <v>47</v>
+      </c>
+      <c r="G2" s="40" t="s">
+        <v>129</v>
+      </c>
+      <c r="H2" s="55" t="s">
+        <v>128</v>
+      </c>
+      <c r="J2" s="39" t="s">
+        <v>46</v>
+      </c>
+      <c r="K2" s="37" t="s">
+        <v>45</v>
+      </c>
+      <c r="L2" s="37" t="s">
+        <v>44</v>
+      </c>
+      <c r="M2" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="N2" s="36" t="s">
+        <v>42</v>
+      </c>
+      <c r="O2" s="37" t="s">
+        <v>41</v>
+      </c>
+      <c r="P2" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q2" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="R2" s="37" t="s">
+        <v>38</v>
+      </c>
+      <c r="S2" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="T2" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="U2" s="35" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A3" s="59" t="s">
+        <v>236</v>
+      </c>
+      <c r="B3" s="29" t="s">
+        <v>262</v>
+      </c>
+      <c r="C3" s="24"/>
+      <c r="D3" s="33" t="s">
+        <v>127</v>
+      </c>
+      <c r="E3" s="27" t="s">
+        <v>127</v>
+      </c>
+      <c r="F3" s="30" t="s">
+        <v>127</v>
+      </c>
+      <c r="G3" s="52"/>
+      <c r="H3" s="29"/>
+      <c r="J3" s="21" t="str">
+        <f>VLOOKUP(D3,[1]!Dictionary[#All],3,FALSE)</f>
+        <v>Body</v>
+      </c>
+      <c r="K3" s="20" t="str">
+        <f>VLOOKUP(D3,[1]!Dictionary[#All],4,FALSE)</f>
+        <v>BODY</v>
+      </c>
+      <c r="L3" s="20" t="str">
+        <f>VLOOKUP(D3,[1]!Dictionary[#All],5,FALSE)</f>
+        <v>99VMS_STRUCTCODE</v>
+      </c>
+      <c r="M3" s="19" t="str">
+        <f>VLOOKUP(D3,[1]!Dictionary[#All],6,FALSE)</f>
+        <v>1.0</v>
+      </c>
+      <c r="N3" s="18" t="str">
+        <f>VLOOKUP(D3,[1]!VolumeType[#All],2,FALSE)</f>
+        <v>Special</v>
+      </c>
+      <c r="O3" s="17" t="str">
+        <f>VLOOKUP(D3,[1]!VolumeType[#All],3,FALSE)</f>
+        <v>BODY</v>
+      </c>
+      <c r="P3" s="16" t="str">
+        <f>VLOOKUP(D3,[1]!Colors[#All],3,FALSE)</f>
+        <v>z Body</v>
+      </c>
+      <c r="Q3" s="14" t="str">
+        <f>IFERROR(VLOOKUP(D3,[1]!DVH_lines[#Data],2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="R3" s="15" t="str">
+        <f>IFERROR(VLOOKUP(D3,[1]!DVH_lines[#Data],3,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="S3" s="13" t="str">
+        <f>IFERROR(VLOOKUP(D3,[1]!DVH_lines[#Data],4,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="T3" s="14">
+        <f>IFERROR(VLOOKUP(D3,[1]!SearchCT[#Data],2,FALSE),"")</f>
+        <v>-350</v>
+      </c>
+      <c r="U3" s="13">
+        <f>IFERROR(VLOOKUP(D3,[1]!SearchCT[#Data],3,FALSE),"")</f>
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A4" s="59" t="s">
+        <v>238</v>
+      </c>
+      <c r="B4" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="24"/>
+      <c r="D4" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="E4" s="27" t="s">
+        <v>126</v>
+      </c>
+      <c r="F4" s="30" t="s">
+        <v>125</v>
+      </c>
+      <c r="G4" s="52"/>
+      <c r="H4" s="29"/>
+      <c r="J4" s="21" t="str">
+        <f>VLOOKUP(D4,[1]!Dictionary[#All],3,FALSE)</f>
+        <v>Treated Volume</v>
+      </c>
+      <c r="K4" s="20" t="str">
+        <f>VLOOKUP(D4,[1]!Dictionary[#All],4,FALSE)</f>
+        <v>Treated Volume</v>
+      </c>
+      <c r="L4" s="20" t="str">
+        <f>VLOOKUP(D4,[1]!Dictionary[#All],5,FALSE)</f>
+        <v>99VMS_STRUCTCODE</v>
+      </c>
+      <c r="M4" s="19" t="str">
+        <f>VLOOKUP(D4,[1]!Dictionary[#All],6,FALSE)</f>
+        <v>1.0</v>
+      </c>
+      <c r="N4" s="18" t="str">
+        <f>VLOOKUP(D4,[1]!VolumeType[#All],2,FALSE)</f>
+        <v>Special</v>
+      </c>
+      <c r="O4" s="17" t="str">
+        <f>VLOOKUP(D4,[1]!VolumeType[#All],3,FALSE)</f>
+        <v>PTV</v>
+      </c>
+      <c r="P4" s="16" t="str">
+        <f>VLOOKUP(D4,[1]!Colors[#All],3,FALSE)</f>
+        <v>z DPV</v>
+      </c>
+      <c r="Q4" s="14" t="str">
+        <f>IFERROR(VLOOKUP(D4,[1]!DVH_lines[#Data],2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="R4" s="15" t="str">
+        <f>IFERROR(VLOOKUP(D4,[1]!DVH_lines[#Data],3,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="S4" s="13" t="str">
+        <f>IFERROR(VLOOKUP(D4,[1]!DVH_lines[#Data],4,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="T4" s="14" t="str">
+        <f>IFERROR(VLOOKUP(D4,[1]!SearchCT[#Data],2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="U4" s="13" t="str">
+        <f>IFERROR(VLOOKUP(D4,[1]!SearchCT[#Data],3,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A5" s="59" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="29" t="s">
+        <v>263</v>
+      </c>
+      <c r="C5" s="24"/>
+      <c r="D5" s="33" t="s">
+        <v>121</v>
+      </c>
+      <c r="E5" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="F5" s="30" t="s">
+        <v>121</v>
+      </c>
+      <c r="G5" s="52"/>
+      <c r="H5" s="29"/>
+      <c r="J5" s="21" t="str">
+        <f>VLOOKUP(D5,[1]!Dictionary[#All],3,FALSE)</f>
+        <v>GTV Primary</v>
+      </c>
+      <c r="K5" s="20" t="str">
+        <f>VLOOKUP(D5,[1]!Dictionary[#All],4,FALSE)</f>
+        <v>GTVp</v>
+      </c>
+      <c r="L5" s="20" t="str">
+        <f>VLOOKUP(D5,[1]!Dictionary[#All],5,FALSE)</f>
+        <v>99VMS_STRUCTCODE</v>
+      </c>
+      <c r="M5" s="19" t="str">
+        <f>VLOOKUP(D5,[1]!Dictionary[#All],6,FALSE)</f>
+        <v>1.0</v>
+      </c>
+      <c r="N5" s="18" t="str">
+        <f>VLOOKUP(D5,[1]!VolumeType[#All],2,FALSE)</f>
+        <v>GTV</v>
+      </c>
+      <c r="O5" s="17" t="str">
+        <f>VLOOKUP(D5,[1]!VolumeType[#All],3,FALSE)</f>
+        <v>GTV</v>
+      </c>
+      <c r="P5" s="16" t="str">
+        <f>VLOOKUP(D5,[1]!Colors[#All],3,FALSE)</f>
+        <v>z GTV</v>
+      </c>
+      <c r="Q5" s="14" t="str">
+        <f>IFERROR(VLOOKUP(D5,[1]!DVH_lines[#Data],2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="R5" s="15" t="str">
+        <f>IFERROR(VLOOKUP(D5,[1]!DVH_lines[#Data],3,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="S5" s="13" t="str">
+        <f>IFERROR(VLOOKUP(D5,[1]!DVH_lines[#Data],4,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="T5" s="14" t="str">
+        <f>IFERROR(VLOOKUP(D5,[1]!SearchCT[#Data],2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="U5" s="13" t="str">
+        <f>IFERROR(VLOOKUP(D5,[1]!SearchCT[#Data],3,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A6" s="59" t="s">
+        <v>226</v>
+      </c>
+      <c r="B6" s="29">
+        <v>5</v>
+      </c>
+      <c r="C6" s="24"/>
+      <c r="D6" s="33" t="s">
+        <v>120</v>
+      </c>
+      <c r="E6" s="27" t="s">
+        <v>120</v>
+      </c>
+      <c r="F6" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="G6" s="52"/>
+      <c r="H6" s="29"/>
+      <c r="J6" s="21" t="str">
+        <f>VLOOKUP(D6,[1]!Dictionary[#All],3,FALSE)</f>
+        <v>CTV Primary</v>
+      </c>
+      <c r="K6" s="20" t="str">
+        <f>VLOOKUP(D6,[1]!Dictionary[#All],4,FALSE)</f>
+        <v>CTVp</v>
+      </c>
+      <c r="L6" s="20" t="str">
+        <f>VLOOKUP(D6,[1]!Dictionary[#All],5,FALSE)</f>
+        <v>99VMS_STRUCTCODE</v>
+      </c>
+      <c r="M6" s="19" t="str">
+        <f>VLOOKUP(D6,[1]!Dictionary[#All],6,FALSE)</f>
+        <v>1.0</v>
+      </c>
+      <c r="N6" s="18" t="str">
+        <f>VLOOKUP(D6,[1]!VolumeType[#All],2,FALSE)</f>
+        <v>CTV</v>
+      </c>
+      <c r="O6" s="17" t="str">
+        <f>VLOOKUP(D6,[1]!VolumeType[#All],3,FALSE)</f>
+        <v>CTV</v>
+      </c>
+      <c r="P6" s="16" t="str">
+        <f>VLOOKUP(D6,[1]!Colors[#All],3,FALSE)</f>
+        <v>z CTV</v>
+      </c>
+      <c r="Q6" s="14" t="str">
+        <f>IFERROR(VLOOKUP(D6,[1]!DVH_lines[#Data],2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="R6" s="15" t="str">
+        <f>IFERROR(VLOOKUP(D6,[1]!DVH_lines[#Data],3,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="S6" s="13" t="str">
+        <f>IFERROR(VLOOKUP(D6,[1]!DVH_lines[#Data],4,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="T6" s="14" t="str">
+        <f>IFERROR(VLOOKUP(D6,[1]!SearchCT[#Data],2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="U6" s="13" t="str">
+        <f>IFERROR(VLOOKUP(D6,[1]!SearchCT[#Data],3,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A7" s="59" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="32"/>
+      <c r="D7" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="E7" s="27" t="s">
+        <v>117</v>
+      </c>
+      <c r="F7" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="G7" s="52"/>
+      <c r="H7" s="29"/>
+      <c r="J7" s="21" t="str">
+        <f>VLOOKUP(D7,[1]!Dictionary[#All],3,FALSE)</f>
+        <v>PTV Primary</v>
+      </c>
+      <c r="K7" s="20" t="str">
+        <f>VLOOKUP(D7,[1]!Dictionary[#All],4,FALSE)</f>
+        <v>PTVp</v>
+      </c>
+      <c r="L7" s="20" t="str">
+        <f>VLOOKUP(D7,[1]!Dictionary[#All],5,FALSE)</f>
+        <v>99VMS_STRUCTCODE</v>
+      </c>
+      <c r="M7" s="19" t="str">
+        <f>VLOOKUP(D7,[1]!Dictionary[#All],6,FALSE)</f>
+        <v>1.0</v>
+      </c>
+      <c r="N7" s="18" t="str">
+        <f>VLOOKUP(D7,[1]!VolumeType[#All],2,FALSE)</f>
+        <v>PTV</v>
+      </c>
+      <c r="O7" s="17" t="str">
+        <f>VLOOKUP(D7,[1]!VolumeType[#All],3,FALSE)</f>
+        <v>PTV</v>
+      </c>
+      <c r="P7" s="16" t="str">
+        <f>VLOOKUP(D7,[1]!Colors[#All],3,FALSE)</f>
+        <v>z PTV</v>
+      </c>
+      <c r="Q7" s="14" t="str">
+        <f>IFERROR(VLOOKUP(D7,[1]!DVH_lines[#Data],2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="R7" s="15" t="str">
+        <f>IFERROR(VLOOKUP(D7,[1]!DVH_lines[#Data],3,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="S7" s="13" t="str">
+        <f>IFERROR(VLOOKUP(D7,[1]!DVH_lines[#Data],4,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="T7" s="14" t="str">
+        <f>IFERROR(VLOOKUP(D7,[1]!SearchCT[#Data],2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="U7" s="13" t="str">
+        <f>IFERROR(VLOOKUP(D7,[1]!SearchCT[#Data],3,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A8" s="59" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="31" t="s">
+        <v>264</v>
+      </c>
+      <c r="D8" s="72" t="s">
+        <v>117</v>
+      </c>
+      <c r="E8" s="73" t="s">
+        <v>134</v>
+      </c>
+      <c r="F8" s="74" t="s">
+        <v>252</v>
+      </c>
+      <c r="G8" s="75"/>
+      <c r="H8" s="76"/>
+      <c r="J8" s="21" t="str">
+        <f>VLOOKUP(D8,[1]!Dictionary[#All],3,FALSE)</f>
+        <v>PTV Primary</v>
+      </c>
+      <c r="K8" s="20" t="str">
+        <f>VLOOKUP(D8,[1]!Dictionary[#All],4,FALSE)</f>
+        <v>PTVp</v>
+      </c>
+      <c r="L8" s="20" t="str">
+        <f>VLOOKUP(D8,[1]!Dictionary[#All],5,FALSE)</f>
+        <v>99VMS_STRUCTCODE</v>
+      </c>
+      <c r="M8" s="19" t="str">
+        <f>VLOOKUP(D8,[1]!Dictionary[#All],6,FALSE)</f>
+        <v>1.0</v>
+      </c>
+      <c r="N8" s="18" t="str">
+        <f>VLOOKUP(D8,[1]!VolumeType[#All],2,FALSE)</f>
+        <v>PTV</v>
+      </c>
+      <c r="O8" s="17" t="str">
+        <f>VLOOKUP(D8,[1]!VolumeType[#All],3,FALSE)</f>
+        <v>PTV</v>
+      </c>
+      <c r="P8" s="16" t="str">
+        <f>VLOOKUP(D8,[1]!Colors[#All],3,FALSE)</f>
+        <v>z PTV</v>
+      </c>
+      <c r="Q8" s="14" t="str">
+        <f>IFERROR(VLOOKUP(D8,[1]!DVH_lines[#Data],2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="R8" s="15" t="str">
+        <f>IFERROR(VLOOKUP(D8,[1]!DVH_lines[#Data],3,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="S8" s="13" t="str">
+        <f>IFERROR(VLOOKUP(D8,[1]!DVH_lines[#Data],4,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="T8" s="14" t="str">
+        <f>IFERROR(VLOOKUP(D8,[1]!SearchCT[#Data],2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="U8" s="13" t="str">
+        <f>IFERROR(VLOOKUP(D8,[1]!SearchCT[#Data],3,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A9" s="59" t="s">
+        <v>237</v>
+      </c>
+      <c r="B9" s="32" t="s">
+        <v>227</v>
+      </c>
+      <c r="D9" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="27" t="s">
+        <v>260</v>
+      </c>
+      <c r="F9" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="G9" s="52"/>
+      <c r="H9" s="29"/>
+      <c r="J9" s="21" t="str">
+        <f>VLOOKUP(D9,[1]!Dictionary[#All],3,FALSE)</f>
+        <v>Spinal cord</v>
+      </c>
+      <c r="K9" s="20">
+        <f>VLOOKUP(D9,[1]!Dictionary[#All],4,FALSE)</f>
+        <v>7647</v>
+      </c>
+      <c r="L9" s="20" t="str">
+        <f>VLOOKUP(D9,[1]!Dictionary[#All],5,FALSE)</f>
+        <v>FMA</v>
+      </c>
+      <c r="M9" s="19" t="str">
+        <f>VLOOKUP(D9,[1]!Dictionary[#All],6,FALSE)</f>
+        <v>3.2</v>
+      </c>
+      <c r="N9" s="18" t="str">
+        <f>VLOOKUP(D9,[1]!VolumeType[#All],2,FALSE)</f>
+        <v>Organ</v>
+      </c>
+      <c r="O9" s="17" t="str">
+        <f>VLOOKUP(D9,[1]!VolumeType[#All],3,FALSE)</f>
+        <v>Organ</v>
+      </c>
+      <c r="P9" s="16" t="str">
+        <f>VLOOKUP(D9,[1]!Colors[#All],3,FALSE)</f>
+        <v>z Spinal Canal</v>
+      </c>
+      <c r="Q9" s="14" t="str">
+        <f>IFERROR(VLOOKUP(D9,[1]!DVH_lines[#Data],2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="R9" s="15" t="str">
+        <f>IFERROR(VLOOKUP(D9,[1]!DVH_lines[#Data],3,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="S9" s="13" t="str">
+        <f>IFERROR(VLOOKUP(D9,[1]!DVH_lines[#Data],4,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="T9" s="14">
+        <f>IFERROR(VLOOKUP(D9,[1]!SearchCT[#Data],2,FALSE),"")</f>
+        <v>20</v>
+      </c>
+      <c r="U9" s="13">
+        <f>IFERROR(VLOOKUP(D9,[1]!SearchCT[#Data],3,FALSE),"")</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A10" s="59" t="s">
+        <v>224</v>
+      </c>
+      <c r="B10" s="32" t="s">
+        <v>225</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>261</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>254</v>
+      </c>
+      <c r="G10" s="52"/>
+      <c r="H10" s="29"/>
+      <c r="J10" s="21" t="str">
+        <f>VLOOKUP(D10,[1]!Dictionary[#All],3,FALSE)</f>
+        <v>PRV</v>
+      </c>
+      <c r="K10" s="20" t="str">
+        <f>VLOOKUP(D10,[1]!Dictionary[#All],4,FALSE)</f>
+        <v>PRV</v>
+      </c>
+      <c r="L10" s="20" t="str">
+        <f>VLOOKUP(D10,[1]!Dictionary[#All],5,FALSE)</f>
+        <v>99VMS_STRUCTCODE</v>
+      </c>
+      <c r="M10" s="19" t="str">
+        <f>VLOOKUP(D10,[1]!Dictionary[#All],6,FALSE)</f>
+        <v>1.0</v>
+      </c>
+      <c r="N10" s="18" t="str">
+        <f>VLOOKUP(D10,[1]!VolumeType[#All],2,FALSE)</f>
+        <v>Control</v>
+      </c>
+      <c r="O10" s="17" t="str">
+        <f>VLOOKUP(D10,[1]!VolumeType[#All],3,FALSE)</f>
+        <v>Avoidance</v>
+      </c>
+      <c r="P10" s="16" t="str">
+        <f>VLOOKUP(D10,[1]!Colors[#All],3,FALSE)</f>
+        <v>zSpinalCanal PRV</v>
+      </c>
+      <c r="Q10" s="14" t="str">
+        <f>IFERROR(VLOOKUP(D10,[1]!DVH_lines[#Data],2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="R10" s="15" t="str">
+        <f>IFERROR(VLOOKUP(D10,[1]!DVH_lines[#Data],3,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="S10" s="13" t="str">
+        <f>IFERROR(VLOOKUP(D10,[1]!DVH_lines[#Data],4,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="T10" s="14" t="str">
+        <f>IFERROR(VLOOKUP(D10,[1]!SearchCT[#Data],2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="U10" s="13" t="str">
+        <f>IFERROR(VLOOKUP(D10,[1]!SearchCT[#Data],3,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A11" s="59" t="s">
+        <v>247</v>
+      </c>
+      <c r="B11" s="32" t="s">
+        <v>265</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>269</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>270</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>271</v>
+      </c>
+      <c r="G11" s="52"/>
+      <c r="H11" s="29"/>
+      <c r="J11" s="21" t="str">
+        <f>VLOOKUP(D11,[1]!Dictionary[#All],3,FALSE)</f>
+        <v>Control Region</v>
+      </c>
+      <c r="K11" s="20" t="str">
+        <f>VLOOKUP(D11,[1]!Dictionary[#All],4,FALSE)</f>
+        <v>Control</v>
+      </c>
+      <c r="L11" s="20" t="str">
+        <f>VLOOKUP(D11,[1]!Dictionary[#All],5,FALSE)</f>
+        <v>99VMS_STRUCTCODE</v>
+      </c>
+      <c r="M11" s="19" t="str">
+        <f>VLOOKUP(D11,[1]!Dictionary[#All],6,FALSE)</f>
+        <v>1.0</v>
+      </c>
+      <c r="N11" s="18" t="str">
+        <f>VLOOKUP(D11,[1]!VolumeType[#All],2,FALSE)</f>
+        <v>Control</v>
+      </c>
+      <c r="O11" s="17" t="str">
+        <f>VLOOKUP(D11,[1]!VolumeType[#All],3,FALSE)</f>
+        <v>Control</v>
+      </c>
+      <c r="P11" s="16" t="str">
+        <f>VLOOKUP(D11,[1]!Colors[#All],3,FALSE)</f>
+        <v>z Control</v>
+      </c>
+      <c r="Q11" s="14" t="str">
+        <f>IFERROR(VLOOKUP(D11,[1]!DVH_lines[#Data],2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="R11" s="15" t="str">
+        <f>IFERROR(VLOOKUP(D11,[1]!DVH_lines[#Data],3,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="S11" s="13" t="str">
+        <f>IFERROR(VLOOKUP(D11,[1]!DVH_lines[#Data],4,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="T11" s="14" t="str">
+        <f>IFERROR(VLOOKUP(D11,[1]!SearchCT[#Data],2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="U11" s="13" t="str">
+        <f>IFERROR(VLOOKUP(D11,[1]!SearchCT[#Data],3,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A12" s="59" t="s">
+        <v>235</v>
+      </c>
+      <c r="B12" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="E12" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="F12" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="G12" s="52"/>
+      <c r="H12" s="29"/>
+      <c r="J12" s="21" t="str">
+        <f>VLOOKUP(D12,[1]!Dictionary[#All],3,FALSE)</f>
+        <v>Esophagus</v>
+      </c>
+      <c r="K12" s="20">
+        <f>VLOOKUP(D12,[1]!Dictionary[#All],4,FALSE)</f>
+        <v>7131</v>
+      </c>
+      <c r="L12" s="20" t="str">
+        <f>VLOOKUP(D12,[1]!Dictionary[#All],5,FALSE)</f>
+        <v>FMA</v>
+      </c>
+      <c r="M12" s="19" t="str">
+        <f>VLOOKUP(D12,[1]!Dictionary[#All],6,FALSE)</f>
+        <v>3.2</v>
+      </c>
+      <c r="N12" s="18" t="str">
+        <f>VLOOKUP(D12,[1]!VolumeType[#All],2,FALSE)</f>
+        <v>Organ</v>
+      </c>
+      <c r="O12" s="17" t="str">
+        <f>VLOOKUP(D12,[1]!VolumeType[#All],3,FALSE)</f>
+        <v>Organ</v>
+      </c>
+      <c r="P12" s="16" t="str">
+        <f>VLOOKUP(D12,[1]!Colors[#All],3,FALSE)</f>
+        <v>z Esophagus</v>
+      </c>
+      <c r="Q12" s="14" t="str">
+        <f>IFERROR(VLOOKUP(D12,[1]!DVH_lines[#Data],2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="R12" s="15" t="str">
+        <f>IFERROR(VLOOKUP(D12,[1]!DVH_lines[#Data],3,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="S12" s="13" t="str">
+        <f>IFERROR(VLOOKUP(D12,[1]!DVH_lines[#Data],4,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="T12" s="14" t="str">
+        <f>IFERROR(VLOOKUP(D12,[1]!SearchCT[#Data],2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="U12" s="13" t="str">
+        <f>IFERROR(VLOOKUP(D12,[1]!SearchCT[#Data],3,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A13" s="59" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="33"/>
+      <c r="E13" s="27"/>
+      <c r="F13" s="30"/>
+      <c r="G13" s="52"/>
+      <c r="H13" s="29"/>
+      <c r="J13" s="21" t="str">
+        <f>VLOOKUP(D17,[1]!Dictionary[#All],3,FALSE)</f>
+        <v>Aorta</v>
+      </c>
+      <c r="K13" s="20">
+        <f>VLOOKUP(D17,[1]!Dictionary[#All],4,FALSE)</f>
+        <v>3734</v>
+      </c>
+      <c r="L13" s="20" t="str">
+        <f>VLOOKUP(D17,[1]!Dictionary[#All],5,FALSE)</f>
+        <v>FMA</v>
+      </c>
+      <c r="M13" s="19" t="str">
+        <f>VLOOKUP(D17,[1]!Dictionary[#All],6,FALSE)</f>
+        <v>3.2</v>
+      </c>
+      <c r="N13" s="18" t="str">
+        <f>VLOOKUP(D17,[1]!VolumeType[#All],2,FALSE)</f>
+        <v>Organ</v>
+      </c>
+      <c r="O13" s="17" t="str">
+        <f>VLOOKUP(D17,[1]!VolumeType[#All],3,FALSE)</f>
+        <v>Organ</v>
+      </c>
+      <c r="P13" s="16" t="str">
+        <f>VLOOKUP(D17,[1]!Colors[#All],3,FALSE)</f>
+        <v>z Aorta</v>
+      </c>
+      <c r="Q13" s="14" t="str">
+        <f>IFERROR(VLOOKUP(D17,[1]!DVH_lines[#Data],2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="R13" s="15" t="str">
+        <f>IFERROR(VLOOKUP(D17,[1]!DVH_lines[#Data],3,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="S13" s="13" t="str">
+        <f>IFERROR(VLOOKUP(D17,[1]!DVH_lines[#Data],4,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="T13" s="14" t="str">
+        <f>IFERROR(VLOOKUP(D17,[1]!SearchCT[#Data],2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="U13" s="13" t="str">
+        <f>IFERROR(VLOOKUP(D17,[1]!SearchCT[#Data],3,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A14" s="22"/>
+      <c r="B14" s="22"/>
+      <c r="D14" s="33"/>
+      <c r="E14" s="27"/>
+      <c r="F14" s="30"/>
+      <c r="G14" s="52"/>
+      <c r="H14" s="29"/>
+      <c r="J14" s="21" t="str">
+        <f>VLOOKUP(D18,[1]!Dictionary[#All],3,FALSE)</f>
+        <v>Artifact</v>
+      </c>
+      <c r="K14" s="20">
+        <f>VLOOKUP(D18,[1]!Dictionary[#All],4,FALSE)</f>
+        <v>11296</v>
+      </c>
+      <c r="L14" s="20" t="str">
+        <f>VLOOKUP(D18,[1]!Dictionary[#All],5,FALSE)</f>
+        <v>RADLEX</v>
+      </c>
+      <c r="M14" s="19">
+        <f>VLOOKUP(D18,[1]!Dictionary[#All],6,FALSE)</f>
+        <v>3.8</v>
+      </c>
+      <c r="N14" s="18" t="str">
+        <f>VLOOKUP(D18,[1]!VolumeType[#All],2,FALSE)</f>
+        <v>Artifact</v>
+      </c>
+      <c r="O14" s="17" t="str">
+        <f>VLOOKUP(D18,[1]!VolumeType[#All],3,FALSE)</f>
+        <v>None</v>
+      </c>
+      <c r="P14" s="16" t="str">
+        <f>VLOOKUP(D18,[1]!Colors[#All],3,FALSE)</f>
+        <v>z RO Helper</v>
+      </c>
+      <c r="Q14" s="14" t="str">
+        <f>IFERROR(VLOOKUP(D18,[1]!DVH_lines[#Data],2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="R14" s="15" t="str">
+        <f>IFERROR(VLOOKUP(D18,[1]!DVH_lines[#Data],3,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="S14" s="13" t="str">
+        <f>IFERROR(VLOOKUP(D18,[1]!DVH_lines[#Data],4,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="T14" s="14" t="str">
+        <f>IFERROR(VLOOKUP(D18,[1]!SearchCT[#Data],2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="U14" s="13" t="str">
+        <f>IFERROR(VLOOKUP(D18,[1]!SearchCT[#Data],3,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="D15" s="33"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="30"/>
+      <c r="G15" s="52"/>
+      <c r="H15" s="29"/>
+      <c r="J15" s="21" t="str">
+        <f>VLOOKUP(D19,[1]!Dictionary[#All],3,FALSE)</f>
+        <v>Artifact</v>
+      </c>
+      <c r="K15" s="20">
+        <f>VLOOKUP(D19,[1]!Dictionary[#All],4,FALSE)</f>
+        <v>11296</v>
+      </c>
+      <c r="L15" s="20" t="str">
+        <f>VLOOKUP(D19,[1]!Dictionary[#All],5,FALSE)</f>
+        <v>RADLEX</v>
+      </c>
+      <c r="M15" s="19">
+        <f>VLOOKUP(D19,[1]!Dictionary[#All],6,FALSE)</f>
+        <v>3.8</v>
+      </c>
+      <c r="N15" s="18" t="str">
+        <f>VLOOKUP(D19,[1]!VolumeType[#All],2,FALSE)</f>
+        <v>Artifact</v>
+      </c>
+      <c r="O15" s="17" t="str">
+        <f>VLOOKUP(D19,[1]!VolumeType[#All],3,FALSE)</f>
+        <v>None</v>
+      </c>
+      <c r="P15" s="16" t="str">
+        <f>VLOOKUP(D19,[1]!Colors[#All],3,FALSE)</f>
+        <v>z RO Helper</v>
+      </c>
+      <c r="Q15" s="14" t="str">
+        <f>IFERROR(VLOOKUP(D19,[1]!DVH_lines[#Data],2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="R15" s="15" t="str">
+        <f>IFERROR(VLOOKUP(D19,[1]!DVH_lines[#Data],3,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="S15" s="13" t="str">
+        <f>IFERROR(VLOOKUP(D19,[1]!DVH_lines[#Data],4,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="T15" s="14" t="str">
+        <f>IFERROR(VLOOKUP(D19,[1]!SearchCT[#Data],2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="U15" s="13" t="str">
+        <f>IFERROR(VLOOKUP(D19,[1]!SearchCT[#Data],3,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D16" s="33"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="52"/>
+      <c r="H16" s="29"/>
+      <c r="J16" s="10" t="str">
+        <f>VLOOKUP(D20,[1]!Dictionary[#All],3,FALSE)</f>
+        <v>Artifact</v>
+      </c>
+      <c r="K16" s="9">
+        <f>VLOOKUP(D20,[1]!Dictionary[#All],4,FALSE)</f>
+        <v>11296</v>
+      </c>
+      <c r="L16" s="9" t="str">
+        <f>VLOOKUP(D20,[1]!Dictionary[#All],5,FALSE)</f>
+        <v>RADLEX</v>
+      </c>
+      <c r="M16" s="8">
+        <f>VLOOKUP(D20,[1]!Dictionary[#All],6,FALSE)</f>
+        <v>3.8</v>
+      </c>
+      <c r="N16" s="7" t="str">
+        <f>VLOOKUP(D20,[1]!VolumeType[#All],2,FALSE)</f>
+        <v>Artifact</v>
+      </c>
+      <c r="O16" s="6" t="str">
+        <f>VLOOKUP(D20,[1]!VolumeType[#All],3,FALSE)</f>
+        <v>None</v>
+      </c>
+      <c r="P16" s="47" t="str">
+        <f>VLOOKUP(D20,[1]!Colors[#All],3,FALSE)</f>
+        <v>z RO Helper</v>
+      </c>
+      <c r="Q16" s="3" t="str">
+        <f>IFERROR(VLOOKUP(D20,[1]!DVH_lines[#Data],2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="R16" s="4" t="str">
+        <f>IFERROR(VLOOKUP(D20,[1]!DVH_lines[#Data],3,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="S16" s="2" t="str">
+        <f>IFERROR(VLOOKUP(D20,[1]!DVH_lines[#Data],4,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="T16" s="3" t="str">
+        <f>IFERROR(VLOOKUP(D20,[1]!SearchCT[#Data],2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="U16" s="2" t="str">
+        <f>IFERROR(VLOOKUP(D20,[1]!SearchCT[#Data],3,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D17" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="G17" s="52"/>
+      <c r="H17" s="29"/>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D18" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="E18" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="F18" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="G18" s="52"/>
+      <c r="H18" s="29"/>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D19" s="33" t="s">
+        <v>109</v>
+      </c>
+      <c r="E19" s="27" t="s">
+        <v>110</v>
+      </c>
+      <c r="F19" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="G19" s="52"/>
+      <c r="H19" s="29"/>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B20"/>
+      <c r="D20" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="E20" s="27" t="s">
+        <v>108</v>
+      </c>
+      <c r="F20" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="G20" s="52"/>
+      <c r="H20" s="29"/>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B21"/>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B22"/>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B23"/>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B24"/>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B25"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:H1"/>
+    <mergeCell ref="J1:M1"/>
+    <mergeCell ref="N1:O1"/>
+    <mergeCell ref="Q1:S1"/>
+    <mergeCell ref="T1:U1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="93" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <tableParts count="2">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:U25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.5703125" style="59" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.42578125" style="59" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.42578125" style="59" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" style="59" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" style="59" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.42578125" style="59" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" style="59" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.85546875" style="59" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.85546875" style="59" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25.28515625" style="59" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.42578125" style="59" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.7109375" style="59" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21" style="59" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.7109375" style="59" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.42578125" style="59" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.28515625" style="59" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.42578125" style="59" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.140625" style="59" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.42578125" style="59" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14" style="59" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.42578125" style="59" bestFit="1" customWidth="1"/>
+    <col min="22" max="16384" width="9.140625" style="59"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="62" t="s">
+        <v>266</v>
+      </c>
+      <c r="B1" s="62"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="62" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="62"/>
+      <c r="H1" s="62"/>
+      <c r="J1" s="60" t="s">
+        <v>54</v>
+      </c>
+      <c r="K1" s="63"/>
+      <c r="L1" s="63"/>
+      <c r="M1" s="61"/>
+      <c r="N1" s="60" t="s">
+        <v>53</v>
+      </c>
+      <c r="O1" s="63"/>
+      <c r="P1" s="51" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q1" s="60" t="s">
+        <v>51</v>
+      </c>
+      <c r="R1" s="63"/>
+      <c r="S1" s="61"/>
+      <c r="T1" s="60" t="s">
+        <v>50</v>
+      </c>
+      <c r="U1" s="61"/>
+    </row>
+    <row r="2" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="42" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" s="50" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="24"/>
+      <c r="D2" s="42" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="41" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" s="40" t="s">
+        <v>47</v>
+      </c>
+      <c r="G2" s="40" t="s">
+        <v>129</v>
+      </c>
+      <c r="H2" s="55" t="s">
+        <v>128</v>
+      </c>
+      <c r="J2" s="39" t="s">
+        <v>46</v>
+      </c>
+      <c r="K2" s="37" t="s">
+        <v>45</v>
+      </c>
+      <c r="L2" s="37" t="s">
+        <v>44</v>
+      </c>
+      <c r="M2" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="N2" s="36" t="s">
+        <v>42</v>
+      </c>
+      <c r="O2" s="37" t="s">
+        <v>41</v>
+      </c>
+      <c r="P2" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q2" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="R2" s="37" t="s">
+        <v>38</v>
+      </c>
+      <c r="S2" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="T2" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="U2" s="35" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A3" s="59" t="s">
+        <v>236</v>
+      </c>
+      <c r="B3" s="29" t="s">
+        <v>266</v>
+      </c>
+      <c r="C3" s="24"/>
+      <c r="D3" s="33" t="s">
+        <v>127</v>
+      </c>
+      <c r="E3" s="27" t="s">
+        <v>127</v>
+      </c>
+      <c r="F3" s="30" t="s">
+        <v>127</v>
+      </c>
+      <c r="G3" s="52"/>
+      <c r="H3" s="29"/>
+      <c r="J3" s="21" t="str">
+        <f>VLOOKUP(D3,[1]!Dictionary[#All],3,FALSE)</f>
+        <v>Body</v>
+      </c>
+      <c r="K3" s="20" t="str">
+        <f>VLOOKUP(D3,[1]!Dictionary[#All],4,FALSE)</f>
+        <v>BODY</v>
+      </c>
+      <c r="L3" s="20" t="str">
+        <f>VLOOKUP(D3,[1]!Dictionary[#All],5,FALSE)</f>
+        <v>99VMS_STRUCTCODE</v>
+      </c>
+      <c r="M3" s="19" t="str">
+        <f>VLOOKUP(D3,[1]!Dictionary[#All],6,FALSE)</f>
+        <v>1.0</v>
+      </c>
+      <c r="N3" s="18" t="str">
+        <f>VLOOKUP(D3,[1]!VolumeType[#All],2,FALSE)</f>
+        <v>Special</v>
+      </c>
+      <c r="O3" s="17" t="str">
+        <f>VLOOKUP(D3,[1]!VolumeType[#All],3,FALSE)</f>
+        <v>BODY</v>
+      </c>
+      <c r="P3" s="16" t="str">
+        <f>VLOOKUP(D3,[1]!Colors[#All],3,FALSE)</f>
+        <v>z Body</v>
+      </c>
+      <c r="Q3" s="14" t="str">
+        <f>IFERROR(VLOOKUP(D3,[1]!DVH_lines[#Data],2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="R3" s="15" t="str">
+        <f>IFERROR(VLOOKUP(D3,[1]!DVH_lines[#Data],3,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="S3" s="13" t="str">
+        <f>IFERROR(VLOOKUP(D3,[1]!DVH_lines[#Data],4,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="T3" s="14">
+        <f>IFERROR(VLOOKUP(D3,[1]!SearchCT[#Data],2,FALSE),"")</f>
+        <v>-350</v>
+      </c>
+      <c r="U3" s="13">
+        <f>IFERROR(VLOOKUP(D3,[1]!SearchCT[#Data],3,FALSE),"")</f>
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A4" s="59" t="s">
+        <v>238</v>
+      </c>
+      <c r="B4" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="24"/>
+      <c r="D4" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="G4" s="52"/>
+      <c r="H4" s="29"/>
+      <c r="J4" s="21" t="str">
+        <f>VLOOKUP(D4,[1]!Dictionary[#All],3,FALSE)</f>
+        <v>Left lung</v>
+      </c>
+      <c r="K4" s="20">
+        <f>VLOOKUP(D4,[1]!Dictionary[#All],4,FALSE)</f>
+        <v>7310</v>
+      </c>
+      <c r="L4" s="20" t="str">
+        <f>VLOOKUP(D4,[1]!Dictionary[#All],5,FALSE)</f>
+        <v>FMA</v>
+      </c>
+      <c r="M4" s="19" t="str">
+        <f>VLOOKUP(D4,[1]!Dictionary[#All],6,FALSE)</f>
+        <v>3.2</v>
+      </c>
+      <c r="N4" s="18" t="str">
+        <f>VLOOKUP(D4,[1]!VolumeType[#All],2,FALSE)</f>
+        <v>Organ</v>
+      </c>
+      <c r="O4" s="17" t="str">
+        <f>VLOOKUP(D4,[1]!VolumeType[#All],3,FALSE)</f>
+        <v>Organ</v>
+      </c>
+      <c r="P4" s="16" t="str">
+        <f>VLOOKUP(D4,[1]!Colors[#All],3,FALSE)</f>
+        <v>z Lung L</v>
+      </c>
+      <c r="Q4" s="14" t="str">
+        <f>IFERROR(VLOOKUP(D4,[1]!DVH_lines[#Data],2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="R4" s="15" t="str">
+        <f>IFERROR(VLOOKUP(D4,[1]!DVH_lines[#Data],3,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="S4" s="13" t="str">
+        <f>IFERROR(VLOOKUP(D4,[1]!DVH_lines[#Data],4,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="T4" s="14">
+        <f>IFERROR(VLOOKUP(D4,[1]!SearchCT[#Data],2,FALSE),"")</f>
+        <v>-700</v>
+      </c>
+      <c r="U4" s="13">
+        <f>IFERROR(VLOOKUP(D4,[1]!SearchCT[#Data],3,FALSE),"")</f>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A5" s="59" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="29" t="s">
+        <v>267</v>
+      </c>
+      <c r="C5" s="24"/>
+      <c r="D5" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" s="52"/>
+      <c r="H5" s="29"/>
+      <c r="J5" s="21" t="str">
+        <f>VLOOKUP(D5,[1]!Dictionary[#All],3,FALSE)</f>
+        <v>Right lung</v>
+      </c>
+      <c r="K5" s="20">
+        <f>VLOOKUP(D5,[1]!Dictionary[#All],4,FALSE)</f>
+        <v>7309</v>
+      </c>
+      <c r="L5" s="20" t="str">
+        <f>VLOOKUP(D5,[1]!Dictionary[#All],5,FALSE)</f>
+        <v>FMA</v>
+      </c>
+      <c r="M5" s="19" t="str">
+        <f>VLOOKUP(D5,[1]!Dictionary[#All],6,FALSE)</f>
+        <v>3.2</v>
+      </c>
+      <c r="N5" s="18" t="str">
+        <f>VLOOKUP(D5,[1]!VolumeType[#All],2,FALSE)</f>
+        <v>Organ</v>
+      </c>
+      <c r="O5" s="17" t="str">
+        <f>VLOOKUP(D5,[1]!VolumeType[#All],3,FALSE)</f>
+        <v>Organ</v>
+      </c>
+      <c r="P5" s="16" t="str">
+        <f>VLOOKUP(D5,[1]!Colors[#All],3,FALSE)</f>
+        <v>z Lung R</v>
+      </c>
+      <c r="Q5" s="14" t="str">
+        <f>IFERROR(VLOOKUP(D5,[1]!DVH_lines[#Data],2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="R5" s="15" t="str">
+        <f>IFERROR(VLOOKUP(D5,[1]!DVH_lines[#Data],3,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="S5" s="13" t="str">
+        <f>IFERROR(VLOOKUP(D5,[1]!DVH_lines[#Data],4,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="T5" s="14">
+        <f>IFERROR(VLOOKUP(D5,[1]!SearchCT[#Data],2,FALSE),"")</f>
+        <v>-700</v>
+      </c>
+      <c r="U5" s="13">
+        <f>IFERROR(VLOOKUP(D5,[1]!SearchCT[#Data],3,FALSE),"")</f>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A6" s="59" t="s">
+        <v>226</v>
+      </c>
+      <c r="B6" s="29">
+        <v>5</v>
+      </c>
+      <c r="C6" s="24"/>
+      <c r="D6" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" s="52"/>
+      <c r="H6" s="29"/>
+      <c r="J6" s="21" t="str">
+        <f>VLOOKUP(D6,[1]!Dictionary[#All],3,FALSE)</f>
+        <v>Pair of lungs</v>
+      </c>
+      <c r="K6" s="20">
+        <f>VLOOKUP(D6,[1]!Dictionary[#All],4,FALSE)</f>
+        <v>68877</v>
+      </c>
+      <c r="L6" s="20" t="str">
+        <f>VLOOKUP(D6,[1]!Dictionary[#All],5,FALSE)</f>
+        <v>FMA</v>
+      </c>
+      <c r="M6" s="19" t="str">
+        <f>VLOOKUP(D6,[1]!Dictionary[#All],6,FALSE)</f>
+        <v>3.2</v>
+      </c>
+      <c r="N6" s="18" t="str">
+        <f>VLOOKUP(D6,[1]!VolumeType[#All],2,FALSE)</f>
+        <v>Organ</v>
+      </c>
+      <c r="O6" s="17" t="str">
+        <f>VLOOKUP(D6,[1]!VolumeType[#All],3,FALSE)</f>
+        <v>Organ</v>
+      </c>
+      <c r="P6" s="16" t="str">
+        <f>VLOOKUP(D6,[1]!Colors[#All],3,FALSE)</f>
+        <v>z Lung B</v>
+      </c>
+      <c r="Q6" s="14" t="str">
+        <f>IFERROR(VLOOKUP(D6,[1]!DVH_lines[#Data],2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="R6" s="15" t="str">
+        <f>IFERROR(VLOOKUP(D6,[1]!DVH_lines[#Data],3,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="S6" s="13" t="str">
+        <f>IFERROR(VLOOKUP(D6,[1]!DVH_lines[#Data],4,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="T6" s="14">
+        <f>IFERROR(VLOOKUP(D6,[1]!SearchCT[#Data],2,FALSE),"")</f>
+        <v>-700</v>
+      </c>
+      <c r="U6" s="13">
+        <f>IFERROR(VLOOKUP(D6,[1]!SearchCT[#Data],3,FALSE),"")</f>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A7" s="59" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="32"/>
+      <c r="D7" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="52"/>
+      <c r="H7" s="29"/>
+      <c r="J7" s="21" t="str">
+        <f>VLOOKUP(D7,[1]!Dictionary[#All],3,FALSE)</f>
+        <v>Heart</v>
+      </c>
+      <c r="K7" s="20">
+        <f>VLOOKUP(D7,[1]!Dictionary[#All],4,FALSE)</f>
+        <v>7088</v>
+      </c>
+      <c r="L7" s="20" t="str">
+        <f>VLOOKUP(D7,[1]!Dictionary[#All],5,FALSE)</f>
+        <v>FMA</v>
+      </c>
+      <c r="M7" s="19" t="str">
+        <f>VLOOKUP(D7,[1]!Dictionary[#All],6,FALSE)</f>
+        <v>3.2</v>
+      </c>
+      <c r="N7" s="18" t="str">
+        <f>VLOOKUP(D7,[1]!VolumeType[#All],2,FALSE)</f>
+        <v>Organ</v>
+      </c>
+      <c r="O7" s="17" t="str">
+        <f>VLOOKUP(D7,[1]!VolumeType[#All],3,FALSE)</f>
+        <v>Organ</v>
+      </c>
+      <c r="P7" s="16" t="str">
+        <f>VLOOKUP(D7,[1]!Colors[#All],3,FALSE)</f>
+        <v>z Heart</v>
+      </c>
+      <c r="Q7" s="14" t="str">
+        <f>IFERROR(VLOOKUP(D7,[1]!DVH_lines[#Data],2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="R7" s="15" t="str">
+        <f>IFERROR(VLOOKUP(D7,[1]!DVH_lines[#Data],3,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="S7" s="13" t="str">
+        <f>IFERROR(VLOOKUP(D7,[1]!DVH_lines[#Data],4,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="T7" s="14" t="str">
+        <f>IFERROR(VLOOKUP(D7,[1]!SearchCT[#Data],2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="U7" s="13" t="str">
+        <f>IFERROR(VLOOKUP(D7,[1]!SearchCT[#Data],3,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A8" s="59" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="31" t="s">
+        <v>264</v>
+      </c>
+      <c r="D8" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" s="52"/>
+      <c r="H8" s="29"/>
+      <c r="J8" s="21" t="str">
+        <f>VLOOKUP(D8,[1]!Dictionary[#All],3,FALSE)</f>
+        <v>Spinal cord</v>
+      </c>
+      <c r="K8" s="20">
+        <f>VLOOKUP(D8,[1]!Dictionary[#All],4,FALSE)</f>
+        <v>7647</v>
+      </c>
+      <c r="L8" s="20" t="str">
+        <f>VLOOKUP(D8,[1]!Dictionary[#All],5,FALSE)</f>
+        <v>FMA</v>
+      </c>
+      <c r="M8" s="19" t="str">
+        <f>VLOOKUP(D8,[1]!Dictionary[#All],6,FALSE)</f>
+        <v>3.2</v>
+      </c>
+      <c r="N8" s="18" t="str">
+        <f>VLOOKUP(D8,[1]!VolumeType[#All],2,FALSE)</f>
+        <v>Organ</v>
+      </c>
+      <c r="O8" s="17" t="str">
+        <f>VLOOKUP(D8,[1]!VolumeType[#All],3,FALSE)</f>
+        <v>Organ</v>
+      </c>
+      <c r="P8" s="16" t="str">
+        <f>VLOOKUP(D8,[1]!Colors[#All],3,FALSE)</f>
+        <v>z Spinal Canal</v>
+      </c>
+      <c r="Q8" s="14" t="str">
+        <f>IFERROR(VLOOKUP(D8,[1]!DVH_lines[#Data],2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="R8" s="15" t="str">
+        <f>IFERROR(VLOOKUP(D8,[1]!DVH_lines[#Data],3,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="S8" s="13" t="str">
+        <f>IFERROR(VLOOKUP(D8,[1]!DVH_lines[#Data],4,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="T8" s="14">
+        <f>IFERROR(VLOOKUP(D8,[1]!SearchCT[#Data],2,FALSE),"")</f>
+        <v>20</v>
+      </c>
+      <c r="U8" s="13">
+        <f>IFERROR(VLOOKUP(D8,[1]!SearchCT[#Data],3,FALSE),"")</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A9" s="59" t="s">
+        <v>237</v>
+      </c>
+      <c r="B9" s="32" t="s">
+        <v>227</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>253</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>254</v>
+      </c>
+      <c r="G9" s="52"/>
+      <c r="H9" s="29"/>
+      <c r="J9" s="21" t="str">
+        <f>VLOOKUP(D9,[1]!Dictionary[#All],3,FALSE)</f>
+        <v>PRV</v>
+      </c>
+      <c r="K9" s="20" t="str">
+        <f>VLOOKUP(D9,[1]!Dictionary[#All],4,FALSE)</f>
+        <v>PRV</v>
+      </c>
+      <c r="L9" s="20" t="str">
+        <f>VLOOKUP(D9,[1]!Dictionary[#All],5,FALSE)</f>
+        <v>99VMS_STRUCTCODE</v>
+      </c>
+      <c r="M9" s="19" t="str">
+        <f>VLOOKUP(D9,[1]!Dictionary[#All],6,FALSE)</f>
+        <v>1.0</v>
+      </c>
+      <c r="N9" s="18" t="str">
+        <f>VLOOKUP(D9,[1]!VolumeType[#All],2,FALSE)</f>
+        <v>Control</v>
+      </c>
+      <c r="O9" s="17" t="str">
+        <f>VLOOKUP(D9,[1]!VolumeType[#All],3,FALSE)</f>
+        <v>Avoidance</v>
+      </c>
+      <c r="P9" s="16" t="str">
+        <f>VLOOKUP(D9,[1]!Colors[#All],3,FALSE)</f>
+        <v>zSpinalCanal PRV</v>
+      </c>
+      <c r="Q9" s="14" t="str">
+        <f>IFERROR(VLOOKUP(D9,[1]!DVH_lines[#Data],2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="R9" s="15" t="str">
+        <f>IFERROR(VLOOKUP(D9,[1]!DVH_lines[#Data],3,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="S9" s="13" t="str">
+        <f>IFERROR(VLOOKUP(D9,[1]!DVH_lines[#Data],4,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="T9" s="14" t="str">
+        <f>IFERROR(VLOOKUP(D9,[1]!SearchCT[#Data],2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="U9" s="13" t="str">
+        <f>IFERROR(VLOOKUP(D9,[1]!SearchCT[#Data],3,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A10" s="59" t="s">
+        <v>224</v>
+      </c>
+      <c r="B10" s="32" t="s">
+        <v>225</v>
+      </c>
+      <c r="D10" s="53" t="s">
+        <v>77</v>
+      </c>
+      <c r="E10" s="27" t="s">
+        <v>77</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="G10" s="52"/>
+      <c r="H10" s="29"/>
+      <c r="J10" s="21" t="str">
+        <f>VLOOKUP(D10,[1]!Dictionary[#All],3,FALSE)</f>
+        <v>Left kidney</v>
+      </c>
+      <c r="K10" s="20">
+        <f>VLOOKUP(D10,[1]!Dictionary[#All],4,FALSE)</f>
+        <v>7205</v>
+      </c>
+      <c r="L10" s="20" t="str">
+        <f>VLOOKUP(D10,[1]!Dictionary[#All],5,FALSE)</f>
+        <v>FMA</v>
+      </c>
+      <c r="M10" s="19" t="str">
+        <f>VLOOKUP(D10,[1]!Dictionary[#All],6,FALSE)</f>
+        <v>3.2</v>
+      </c>
+      <c r="N10" s="18" t="str">
+        <f>VLOOKUP(D10,[1]!VolumeType[#All],2,FALSE)</f>
+        <v>Organ</v>
+      </c>
+      <c r="O10" s="17" t="str">
+        <f>VLOOKUP(D10,[1]!VolumeType[#All],3,FALSE)</f>
+        <v>Organ</v>
+      </c>
+      <c r="P10" s="16" t="str">
+        <f>VLOOKUP(D10,[1]!Colors[#All],3,FALSE)</f>
+        <v>z Kidney L</v>
+      </c>
+      <c r="Q10" s="14" t="str">
+        <f>IFERROR(VLOOKUP(D10,[1]!DVH_lines[#Data],2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="R10" s="15" t="str">
+        <f>IFERROR(VLOOKUP(D10,[1]!DVH_lines[#Data],3,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="S10" s="13" t="str">
+        <f>IFERROR(VLOOKUP(D10,[1]!DVH_lines[#Data],4,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="T10" s="14" t="str">
+        <f>IFERROR(VLOOKUP(D10,[1]!SearchCT[#Data],2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="U10" s="13" t="str">
+        <f>IFERROR(VLOOKUP(D10,[1]!SearchCT[#Data],3,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A11" s="59" t="s">
+        <v>247</v>
+      </c>
+      <c r="B11" s="32" t="s">
+        <v>268</v>
+      </c>
+      <c r="D11" s="54" t="s">
+        <v>75</v>
+      </c>
+      <c r="E11" s="45" t="s">
+        <v>75</v>
+      </c>
+      <c r="F11" s="46" t="s">
+        <v>74</v>
+      </c>
+      <c r="G11" s="52"/>
+      <c r="H11" s="29"/>
+      <c r="J11" s="21" t="str">
+        <f>VLOOKUP(D11,[1]!Dictionary[#All],3,FALSE)</f>
+        <v>Right kidney</v>
+      </c>
+      <c r="K11" s="20">
+        <f>VLOOKUP(D11,[1]!Dictionary[#All],4,FALSE)</f>
+        <v>7204</v>
+      </c>
+      <c r="L11" s="20" t="str">
+        <f>VLOOKUP(D11,[1]!Dictionary[#All],5,FALSE)</f>
+        <v>FMA</v>
+      </c>
+      <c r="M11" s="19" t="str">
+        <f>VLOOKUP(D11,[1]!Dictionary[#All],6,FALSE)</f>
+        <v>3.2</v>
+      </c>
+      <c r="N11" s="18" t="str">
+        <f>VLOOKUP(D11,[1]!VolumeType[#All],2,FALSE)</f>
+        <v>Organ</v>
+      </c>
+      <c r="O11" s="17" t="str">
+        <f>VLOOKUP(D11,[1]!VolumeType[#All],3,FALSE)</f>
+        <v>Organ</v>
+      </c>
+      <c r="P11" s="16" t="str">
+        <f>VLOOKUP(D11,[1]!Colors[#All],3,FALSE)</f>
+        <v>z Kidney R</v>
+      </c>
+      <c r="Q11" s="14" t="str">
+        <f>IFERROR(VLOOKUP(D11,[1]!DVH_lines[#Data],2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="R11" s="15" t="str">
+        <f>IFERROR(VLOOKUP(D11,[1]!DVH_lines[#Data],3,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="S11" s="13" t="str">
+        <f>IFERROR(VLOOKUP(D11,[1]!DVH_lines[#Data],4,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="T11" s="14" t="str">
+        <f>IFERROR(VLOOKUP(D11,[1]!SearchCT[#Data],2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="U11" s="13" t="str">
+        <f>IFERROR(VLOOKUP(D11,[1]!SearchCT[#Data],3,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A12" s="59" t="s">
+        <v>235</v>
+      </c>
+      <c r="B12" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="53" t="s">
+        <v>73</v>
+      </c>
+      <c r="E12" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="G12" s="52"/>
+      <c r="H12" s="29"/>
+      <c r="J12" s="21" t="str">
+        <f>VLOOKUP(D12,[1]!Dictionary[#All],3,FALSE)</f>
+        <v>Set of kidneys</v>
+      </c>
+      <c r="K12" s="20" t="str">
+        <f>VLOOKUP(D12,[1]!Dictionary[#All],4,FALSE)</f>
+        <v>264815</v>
+      </c>
+      <c r="L12" s="20" t="str">
+        <f>VLOOKUP(D12,[1]!Dictionary[#All],5,FALSE)</f>
+        <v>FMA</v>
+      </c>
+      <c r="M12" s="19" t="str">
+        <f>VLOOKUP(D12,[1]!Dictionary[#All],6,FALSE)</f>
+        <v>3.2</v>
+      </c>
+      <c r="N12" s="18" t="str">
+        <f>VLOOKUP(D12,[1]!VolumeType[#All],2,FALSE)</f>
+        <v>Organ</v>
+      </c>
+      <c r="O12" s="17" t="str">
+        <f>VLOOKUP(D12,[1]!VolumeType[#All],3,FALSE)</f>
+        <v>Organ</v>
+      </c>
+      <c r="P12" s="16" t="str">
+        <f>VLOOKUP(D12,[1]!Colors[#All],3,FALSE)</f>
+        <v>z Kidney B</v>
+      </c>
+      <c r="Q12" s="14" t="str">
+        <f>IFERROR(VLOOKUP(D12,[1]!DVH_lines[#Data],2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="R12" s="15" t="str">
+        <f>IFERROR(VLOOKUP(D12,[1]!DVH_lines[#Data],3,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="S12" s="13" t="str">
+        <f>IFERROR(VLOOKUP(D12,[1]!DVH_lines[#Data],4,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="T12" s="14" t="str">
+        <f>IFERROR(VLOOKUP(D12,[1]!SearchCT[#Data],2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="U12" s="13" t="str">
+        <f>IFERROR(VLOOKUP(D12,[1]!SearchCT[#Data],3,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A13" s="59" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="33" t="s">
+        <v>81</v>
+      </c>
+      <c r="E13" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="F13" s="30" t="s">
+        <v>81</v>
+      </c>
+      <c r="G13" s="52"/>
+      <c r="H13" s="29"/>
+      <c r="J13" s="21" t="str">
+        <f>VLOOKUP(D13,[1]!Dictionary[#All],3,FALSE)</f>
+        <v>Liver</v>
+      </c>
+      <c r="K13" s="20">
+        <f>VLOOKUP(D13,[1]!Dictionary[#All],4,FALSE)</f>
+        <v>7197</v>
+      </c>
+      <c r="L13" s="20" t="str">
+        <f>VLOOKUP(D13,[1]!Dictionary[#All],5,FALSE)</f>
+        <v>FMA</v>
+      </c>
+      <c r="M13" s="19" t="str">
+        <f>VLOOKUP(D13,[1]!Dictionary[#All],6,FALSE)</f>
+        <v>3.2</v>
+      </c>
+      <c r="N13" s="18" t="str">
+        <f>VLOOKUP(D13,[1]!VolumeType[#All],2,FALSE)</f>
+        <v>Organ</v>
+      </c>
+      <c r="O13" s="17" t="str">
+        <f>VLOOKUP(D13,[1]!VolumeType[#All],3,FALSE)</f>
+        <v>Organ</v>
+      </c>
+      <c r="P13" s="16" t="str">
+        <f>VLOOKUP(D13,[1]!Colors[#All],3,FALSE)</f>
+        <v>z Liver</v>
+      </c>
+      <c r="Q13" s="14" t="str">
+        <f>IFERROR(VLOOKUP(D13,[1]!DVH_lines[#Data],2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="R13" s="15" t="str">
+        <f>IFERROR(VLOOKUP(D13,[1]!DVH_lines[#Data],3,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="S13" s="13" t="str">
+        <f>IFERROR(VLOOKUP(D13,[1]!DVH_lines[#Data],4,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="T13" s="14" t="str">
+        <f>IFERROR(VLOOKUP(D13,[1]!SearchCT[#Data],2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="U13" s="13" t="str">
+        <f>IFERROR(VLOOKUP(D13,[1]!SearchCT[#Data],3,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A14" s="22"/>
+      <c r="B14" s="22"/>
+      <c r="D14" s="33" t="s">
+        <v>187</v>
+      </c>
+      <c r="E14" s="27" t="s">
+        <v>187</v>
+      </c>
+      <c r="F14" s="30"/>
+      <c r="G14" s="52"/>
+      <c r="H14" s="29"/>
+      <c r="J14" s="21" t="str">
+        <f>VLOOKUP(D14,[1]!Dictionary[#All],3,FALSE)</f>
+        <v>Skin</v>
+      </c>
+      <c r="K14" s="20">
+        <f>VLOOKUP(D14,[1]!Dictionary[#All],4,FALSE)</f>
+        <v>7163</v>
+      </c>
+      <c r="L14" s="20" t="str">
+        <f>VLOOKUP(D14,[1]!Dictionary[#All],5,FALSE)</f>
+        <v>FMA</v>
+      </c>
+      <c r="M14" s="19" t="str">
+        <f>VLOOKUP(D14,[1]!Dictionary[#All],6,FALSE)</f>
+        <v>3.2</v>
+      </c>
+      <c r="N14" s="18" t="str">
+        <f>VLOOKUP(D14,[1]!VolumeType[#All],2,FALSE)</f>
+        <v>Organ</v>
+      </c>
+      <c r="O14" s="17" t="str">
+        <f>VLOOKUP(D14,[1]!VolumeType[#All],3,FALSE)</f>
+        <v>Organ</v>
+      </c>
+      <c r="P14" s="16" t="str">
+        <f>VLOOKUP(D14,[1]!Colors[#All],3,FALSE)</f>
+        <v>z Skin</v>
+      </c>
+      <c r="Q14" s="14" t="str">
+        <f>IFERROR(VLOOKUP(D14,[1]!DVH_lines[#Data],2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="R14" s="15" t="str">
+        <f>IFERROR(VLOOKUP(D14,[1]!DVH_lines[#Data],3,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="S14" s="13" t="str">
+        <f>IFERROR(VLOOKUP(D14,[1]!DVH_lines[#Data],4,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="T14" s="14" t="str">
+        <f>IFERROR(VLOOKUP(D14,[1]!SearchCT[#Data],2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="U14" s="13" t="str">
+        <f>IFERROR(VLOOKUP(D14,[1]!SearchCT[#Data],3,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="D15" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="F15" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="G15" s="52"/>
+      <c r="H15" s="29"/>
+      <c r="J15" s="21" t="str">
+        <f>VLOOKUP(D15,[1]!Dictionary[#All],3,FALSE)</f>
+        <v>Left brachial nerve plexus</v>
+      </c>
+      <c r="K15" s="20">
+        <f>VLOOKUP(D15,[1]!Dictionary[#All],4,FALSE)</f>
+        <v>45245</v>
+      </c>
+      <c r="L15" s="20" t="str">
+        <f>VLOOKUP(D15,[1]!Dictionary[#All],5,FALSE)</f>
+        <v>FMA</v>
+      </c>
+      <c r="M15" s="19" t="str">
+        <f>VLOOKUP(D15,[1]!Dictionary[#All],6,FALSE)</f>
+        <v>3.2</v>
+      </c>
+      <c r="N15" s="18" t="str">
+        <f>VLOOKUP(D15,[1]!VolumeType[#All],2,FALSE)</f>
+        <v>Organ</v>
+      </c>
+      <c r="O15" s="17" t="str">
+        <f>VLOOKUP(D15,[1]!VolumeType[#All],3,FALSE)</f>
+        <v>Organ</v>
+      </c>
+      <c r="P15" s="16" t="str">
+        <f>VLOOKUP(D15,[1]!Colors[#All],3,FALSE)</f>
+        <v>zBrachialPlexusL</v>
+      </c>
+      <c r="Q15" s="14" t="str">
+        <f>IFERROR(VLOOKUP(D15,[1]!DVH_lines[#Data],2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="R15" s="15" t="str">
+        <f>IFERROR(VLOOKUP(D15,[1]!DVH_lines[#Data],3,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="S15" s="13" t="str">
+        <f>IFERROR(VLOOKUP(D15,[1]!DVH_lines[#Data],4,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="T15" s="14" t="str">
+        <f>IFERROR(VLOOKUP(D15,[1]!SearchCT[#Data],2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="U15" s="13" t="str">
+        <f>IFERROR(VLOOKUP(D15,[1]!SearchCT[#Data],3,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="D16" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="F16" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="G16" s="52"/>
+      <c r="H16" s="29"/>
+      <c r="J16" s="21" t="str">
+        <f>VLOOKUP(D16,[1]!Dictionary[#All],3,FALSE)</f>
+        <v>Right brachial nerve plexus</v>
+      </c>
+      <c r="K16" s="20">
+        <f>VLOOKUP(D16,[1]!Dictionary[#All],4,FALSE)</f>
+        <v>45244</v>
+      </c>
+      <c r="L16" s="20" t="str">
+        <f>VLOOKUP(D16,[1]!Dictionary[#All],5,FALSE)</f>
+        <v>FMA</v>
+      </c>
+      <c r="M16" s="19" t="str">
+        <f>VLOOKUP(D16,[1]!Dictionary[#All],6,FALSE)</f>
+        <v>3.2</v>
+      </c>
+      <c r="N16" s="18" t="str">
+        <f>VLOOKUP(D16,[1]!VolumeType[#All],2,FALSE)</f>
+        <v>Organ</v>
+      </c>
+      <c r="O16" s="17" t="str">
+        <f>VLOOKUP(D16,[1]!VolumeType[#All],3,FALSE)</f>
+        <v>Organ</v>
+      </c>
+      <c r="P16" s="16" t="str">
+        <f>VLOOKUP(D16,[1]!Colors[#All],3,FALSE)</f>
+        <v>zBrachialPlexusR</v>
+      </c>
+      <c r="Q16" s="14" t="str">
+        <f>IFERROR(VLOOKUP(D16,[1]!DVH_lines[#Data],2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="R16" s="15" t="str">
+        <f>IFERROR(VLOOKUP(D16,[1]!DVH_lines[#Data],3,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="S16" s="13" t="str">
+        <f>IFERROR(VLOOKUP(D16,[1]!DVH_lines[#Data],4,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="T16" s="14" t="str">
+        <f>IFERROR(VLOOKUP(D16,[1]!SearchCT[#Data],2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="U16" s="13" t="str">
+        <f>IFERROR(VLOOKUP(D16,[1]!SearchCT[#Data],3,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="D17" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="E17" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="F17" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="G17" s="52"/>
+      <c r="H17" s="29"/>
+      <c r="J17" s="21" t="str">
+        <f>VLOOKUP(D17,[1]!Dictionary[#All],3,FALSE)</f>
+        <v>Trachea</v>
+      </c>
+      <c r="K17" s="20">
+        <f>VLOOKUP(D17,[1]!Dictionary[#All],4,FALSE)</f>
+        <v>7394</v>
+      </c>
+      <c r="L17" s="20" t="str">
+        <f>VLOOKUP(D17,[1]!Dictionary[#All],5,FALSE)</f>
+        <v>FMA</v>
+      </c>
+      <c r="M17" s="19" t="str">
+        <f>VLOOKUP(D17,[1]!Dictionary[#All],6,FALSE)</f>
+        <v>3.2</v>
+      </c>
+      <c r="N17" s="18" t="str">
+        <f>VLOOKUP(D17,[1]!VolumeType[#All],2,FALSE)</f>
+        <v>Organ</v>
+      </c>
+      <c r="O17" s="17" t="str">
+        <f>VLOOKUP(D17,[1]!VolumeType[#All],3,FALSE)</f>
+        <v>Organ</v>
+      </c>
+      <c r="P17" s="16" t="str">
+        <f>VLOOKUP(D17,[1]!Colors[#All],3,FALSE)</f>
+        <v>z Trachea</v>
+      </c>
+      <c r="Q17" s="14" t="str">
+        <f>IFERROR(VLOOKUP(D17,[1]!DVH_lines[#Data],2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="R17" s="15" t="str">
+        <f>IFERROR(VLOOKUP(D17,[1]!DVH_lines[#Data],3,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="S17" s="13" t="str">
+        <f>IFERROR(VLOOKUP(D17,[1]!DVH_lines[#Data],4,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="T17" s="14" t="str">
+        <f>IFERROR(VLOOKUP(D17,[1]!SearchCT[#Data],2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="U17" s="13" t="str">
+        <f>IFERROR(VLOOKUP(D17,[1]!SearchCT[#Data],3,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="D18" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="E18" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="F18" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="G18" s="52"/>
+      <c r="H18" s="29"/>
+      <c r="J18" s="21" t="str">
+        <f>VLOOKUP(D18,[1]!Dictionary[#All],3,FALSE)</f>
+        <v>Bronchial tree</v>
+      </c>
+      <c r="K18" s="20">
+        <f>VLOOKUP(D18,[1]!Dictionary[#All],4,FALSE)</f>
+        <v>26660</v>
+      </c>
+      <c r="L18" s="20" t="str">
+        <f>VLOOKUP(D18,[1]!Dictionary[#All],5,FALSE)</f>
+        <v>FMA</v>
+      </c>
+      <c r="M18" s="19" t="str">
+        <f>VLOOKUP(D18,[1]!Dictionary[#All],6,FALSE)</f>
+        <v>3.2</v>
+      </c>
+      <c r="N18" s="18" t="str">
+        <f>VLOOKUP(D18,[1]!VolumeType[#All],2,FALSE)</f>
+        <v>Organ</v>
+      </c>
+      <c r="O18" s="17" t="str">
+        <f>VLOOKUP(D18,[1]!VolumeType[#All],3,FALSE)</f>
+        <v>Organ</v>
+      </c>
+      <c r="P18" s="16" t="str">
+        <f>VLOOKUP(D18,[1]!Colors[#All],3,FALSE)</f>
+        <v>z BronchialTree</v>
+      </c>
+      <c r="Q18" s="14" t="str">
+        <f>IFERROR(VLOOKUP(D18,[1]!DVH_lines[#Data],2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="R18" s="15" t="str">
+        <f>IFERROR(VLOOKUP(D18,[1]!DVH_lines[#Data],3,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="S18" s="13" t="str">
+        <f>IFERROR(VLOOKUP(D18,[1]!DVH_lines[#Data],4,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="T18" s="14" t="str">
+        <f>IFERROR(VLOOKUP(D18,[1]!SearchCT[#Data],2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="U18" s="13" t="str">
+        <f>IFERROR(VLOOKUP(D18,[1]!SearchCT[#Data],3,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="D19" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="E19" s="27" t="s">
+        <v>80</v>
+      </c>
+      <c r="F19" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="G19" s="52"/>
+      <c r="H19" s="29"/>
+      <c r="J19" s="21" t="str">
+        <f>VLOOKUP(D19,[1]!Dictionary[#All],3,FALSE)</f>
+        <v>Stomach</v>
+      </c>
+      <c r="K19" s="20">
+        <f>VLOOKUP(D19,[1]!Dictionary[#All],4,FALSE)</f>
+        <v>7148</v>
+      </c>
+      <c r="L19" s="20" t="str">
+        <f>VLOOKUP(D19,[1]!Dictionary[#All],5,FALSE)</f>
+        <v>FMA</v>
+      </c>
+      <c r="M19" s="19" t="str">
+        <f>VLOOKUP(D19,[1]!Dictionary[#All],6,FALSE)</f>
+        <v>3.2</v>
+      </c>
+      <c r="N19" s="18" t="str">
+        <f>VLOOKUP(D19,[1]!VolumeType[#All],2,FALSE)</f>
+        <v>Organ</v>
+      </c>
+      <c r="O19" s="17" t="str">
+        <f>VLOOKUP(D19,[1]!VolumeType[#All],3,FALSE)</f>
+        <v>Organ</v>
+      </c>
+      <c r="P19" s="16" t="str">
+        <f>VLOOKUP(D19,[1]!Colors[#All],3,FALSE)</f>
+        <v>z Stomach</v>
+      </c>
+      <c r="Q19" s="14" t="str">
+        <f>IFERROR(VLOOKUP(D19,[1]!DVH_lines[#Data],2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="R19" s="15" t="str">
+        <f>IFERROR(VLOOKUP(D19,[1]!DVH_lines[#Data],3,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="S19" s="13" t="str">
+        <f>IFERROR(VLOOKUP(D19,[1]!DVH_lines[#Data],4,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="T19" s="14" t="str">
+        <f>IFERROR(VLOOKUP(D19,[1]!SearchCT[#Data],2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="U19" s="13" t="str">
+        <f>IFERROR(VLOOKUP(D19,[1]!SearchCT[#Data],3,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B20"/>
+      <c r="D20" t="s">
+        <v>69</v>
+      </c>
+      <c r="E20" t="s">
+        <v>69</v>
+      </c>
+      <c r="F20" t="s">
+        <v>272</v>
+      </c>
+      <c r="G20" s="52"/>
+      <c r="H20" s="29"/>
+      <c r="J20" s="21" t="str">
+        <f>VLOOKUP(D20,[1]!Dictionary[#All],3,FALSE)</f>
+        <v>Small intestine</v>
+      </c>
+      <c r="K20" s="20">
+        <f>VLOOKUP(D20,[1]!Dictionary[#All],4,FALSE)</f>
+        <v>7200</v>
+      </c>
+      <c r="L20" s="20" t="str">
+        <f>VLOOKUP(D20,[1]!Dictionary[#All],5,FALSE)</f>
+        <v>FMA</v>
+      </c>
+      <c r="M20" s="19" t="str">
+        <f>VLOOKUP(D20,[1]!Dictionary[#All],6,FALSE)</f>
+        <v>3.2</v>
+      </c>
+      <c r="N20" s="18" t="str">
+        <f>VLOOKUP(D20,[1]!VolumeType[#All],2,FALSE)</f>
+        <v>Organ</v>
+      </c>
+      <c r="O20" s="17" t="str">
+        <f>VLOOKUP(D20,[1]!VolumeType[#All],3,FALSE)</f>
+        <v>Organ</v>
+      </c>
+      <c r="P20" s="16" t="str">
+        <f>VLOOKUP(D20,[1]!Colors[#All],3,FALSE)</f>
+        <v>z Small Bowel</v>
+      </c>
+      <c r="Q20" s="14" t="str">
+        <f>IFERROR(VLOOKUP(D20,[1]!DVH_lines[#Data],2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="R20" s="15" t="str">
+        <f>IFERROR(VLOOKUP(D20,[1]!DVH_lines[#Data],3,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="S20" s="13" t="str">
+        <f>IFERROR(VLOOKUP(D20,[1]!DVH_lines[#Data],4,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="T20" s="14" t="str">
+        <f>IFERROR(VLOOKUP(D20,[1]!SearchCT[#Data],2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="U20" s="13" t="str">
+        <f>IFERROR(VLOOKUP(D20,[1]!SearchCT[#Data],3,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B21"/>
+      <c r="D21" t="s">
+        <v>70</v>
+      </c>
+      <c r="E21" t="s">
+        <v>70</v>
+      </c>
+      <c r="F21" t="s">
+        <v>273</v>
+      </c>
+      <c r="G21" s="52"/>
+      <c r="H21" s="29"/>
+      <c r="J21" s="21" t="str">
+        <f>VLOOKUP(D21,[1]!Dictionary[#All],3,FALSE)</f>
+        <v>Large intestine</v>
+      </c>
+      <c r="K21" s="20">
+        <f>VLOOKUP(D21,[1]!Dictionary[#All],4,FALSE)</f>
+        <v>7201</v>
+      </c>
+      <c r="L21" s="20" t="str">
+        <f>VLOOKUP(D21,[1]!Dictionary[#All],5,FALSE)</f>
+        <v>FMA</v>
+      </c>
+      <c r="M21" s="19" t="str">
+        <f>VLOOKUP(D21,[1]!Dictionary[#All],6,FALSE)</f>
+        <v>3.2</v>
+      </c>
+      <c r="N21" s="18" t="str">
+        <f>VLOOKUP(D21,[1]!VolumeType[#All],2,FALSE)</f>
+        <v>Organ</v>
+      </c>
+      <c r="O21" s="17" t="str">
+        <f>VLOOKUP(D21,[1]!VolumeType[#All],3,FALSE)</f>
+        <v>Organ</v>
+      </c>
+      <c r="P21" s="16" t="str">
+        <f>VLOOKUP(D21,[1]!Colors[#All],3,FALSE)</f>
+        <v>z Large Bowel</v>
+      </c>
+      <c r="Q21" s="14" t="str">
+        <f>IFERROR(VLOOKUP(D21,[1]!DVH_lines[#Data],2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="R21" s="15" t="str">
+        <f>IFERROR(VLOOKUP(D21,[1]!DVH_lines[#Data],3,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="S21" s="13" t="str">
+        <f>IFERROR(VLOOKUP(D21,[1]!DVH_lines[#Data],4,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="T21" s="14" t="str">
+        <f>IFERROR(VLOOKUP(D21,[1]!SearchCT[#Data],2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="U21" s="13" t="str">
+        <f>IFERROR(VLOOKUP(D21,[1]!SearchCT[#Data],3,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B22"/>
+      <c r="D22" t="s">
+        <v>274</v>
+      </c>
+      <c r="E22" t="s">
+        <v>274</v>
+      </c>
+      <c r="F22" t="s">
+        <v>274</v>
+      </c>
+      <c r="G22" s="52"/>
+      <c r="H22" s="29"/>
+      <c r="J22" s="21" t="str">
+        <f>VLOOKUP(D22,[1]!Dictionary[#All],3,FALSE)</f>
+        <v>Sacral nerve plexus</v>
+      </c>
+      <c r="K22" s="20">
+        <f>VLOOKUP(D22,[1]!Dictionary[#All],4,FALSE)</f>
+        <v>5909</v>
+      </c>
+      <c r="L22" s="20" t="str">
+        <f>VLOOKUP(D22,[1]!Dictionary[#All],5,FALSE)</f>
+        <v>FMA</v>
+      </c>
+      <c r="M22" s="19" t="str">
+        <f>VLOOKUP(D22,[1]!Dictionary[#All],6,FALSE)</f>
+        <v>3.2</v>
+      </c>
+      <c r="N22" s="18" t="str">
+        <f>VLOOKUP(D22,[1]!VolumeType[#All],2,FALSE)</f>
+        <v>Organ</v>
+      </c>
+      <c r="O22" s="17" t="str">
+        <f>VLOOKUP(D22,[1]!VolumeType[#All],3,FALSE)</f>
+        <v>Organ</v>
+      </c>
+      <c r="P22" s="16" t="str">
+        <f>VLOOKUP(D22,[1]!Colors[#All],3,FALSE)</f>
+        <v>z Sacral plexus</v>
+      </c>
+      <c r="Q22" s="14" t="str">
+        <f>IFERROR(VLOOKUP(D22,[1]!DVH_lines[#Data],2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="R22" s="15" t="str">
+        <f>IFERROR(VLOOKUP(D22,[1]!DVH_lines[#Data],3,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="S22" s="13" t="str">
+        <f>IFERROR(VLOOKUP(D22,[1]!DVH_lines[#Data],4,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="T22" s="14" t="str">
+        <f>IFERROR(VLOOKUP(D22,[1]!SearchCT[#Data],2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="U22" s="13" t="str">
+        <f>IFERROR(VLOOKUP(D22,[1]!SearchCT[#Data],3,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B23"/>
+      <c r="D23" t="s">
+        <v>275</v>
+      </c>
+      <c r="E23" t="s">
+        <v>275</v>
+      </c>
+      <c r="F23" t="s">
+        <v>275</v>
+      </c>
+      <c r="G23" s="52"/>
+      <c r="H23" s="29"/>
+      <c r="J23" s="21" t="str">
+        <f>VLOOKUP(D23,[1]!Dictionary[#All],3,FALSE)</f>
+        <v>Urethra</v>
+      </c>
+      <c r="K23" s="20">
+        <f>VLOOKUP(D23,[1]!Dictionary[#All],4,FALSE)</f>
+        <v>19667</v>
+      </c>
+      <c r="L23" s="20" t="str">
+        <f>VLOOKUP(D23,[1]!Dictionary[#All],5,FALSE)</f>
+        <v>FMA</v>
+      </c>
+      <c r="M23" s="19" t="str">
+        <f>VLOOKUP(D23,[1]!Dictionary[#All],6,FALSE)</f>
+        <v>3.2</v>
+      </c>
+      <c r="N23" s="18" t="str">
+        <f>VLOOKUP(D23,[1]!VolumeType[#All],2,FALSE)</f>
+        <v>Organ</v>
+      </c>
+      <c r="O23" s="17" t="str">
+        <f>VLOOKUP(D23,[1]!VolumeType[#All],3,FALSE)</f>
+        <v>Organ</v>
+      </c>
+      <c r="P23" s="16" t="str">
+        <f>VLOOKUP(D23,[1]!Colors[#All],3,FALSE)</f>
+        <v>z Urethra</v>
+      </c>
+      <c r="Q23" s="14" t="str">
+        <f>IFERROR(VLOOKUP(D23,[1]!DVH_lines[#Data],2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="R23" s="15" t="str">
+        <f>IFERROR(VLOOKUP(D23,[1]!DVH_lines[#Data],3,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="S23" s="13" t="str">
+        <f>IFERROR(VLOOKUP(D23,[1]!DVH_lines[#Data],4,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="T23" s="14" t="str">
+        <f>IFERROR(VLOOKUP(D23,[1]!SearchCT[#Data],2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="U23" s="13" t="str">
+        <f>IFERROR(VLOOKUP(D23,[1]!SearchCT[#Data],3,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="24" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B24"/>
+      <c r="D24" s="68" t="s">
+        <v>255</v>
+      </c>
+      <c r="E24" s="69" t="s">
+        <v>256</v>
+      </c>
+      <c r="F24" s="70" t="s">
+        <v>255</v>
+      </c>
+      <c r="G24" s="71" t="str">
+        <f>IF(EXACT(D24,"DPV"),VLOOKUP(REPLACE($B$8,1,1,""),[1]!ICD_Codes[#All],2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="H24" s="31" t="str">
+        <f t="shared" ref="H24:H25" si="0">IF(EXACT(D24,"DPV"),"ICD-10","")</f>
+        <v/>
+      </c>
+      <c r="J24" s="21" t="str">
+        <f>VLOOKUP(D24,[1]!Dictionary[#All],3,FALSE)</f>
+        <v>Brainstem</v>
+      </c>
+      <c r="K24" s="20">
+        <f>VLOOKUP(D24,[1]!Dictionary[#All],4,FALSE)</f>
+        <v>79876</v>
+      </c>
+      <c r="L24" s="20" t="str">
+        <f>VLOOKUP(D24,[1]!Dictionary[#All],5,FALSE)</f>
+        <v>FMA</v>
+      </c>
+      <c r="M24" s="19" t="str">
+        <f>VLOOKUP(D24,[1]!Dictionary[#All],6,FALSE)</f>
+        <v>3.2</v>
+      </c>
+      <c r="N24" s="18" t="str">
+        <f>VLOOKUP(D24,[1]!VolumeType[#All],2,FALSE)</f>
+        <v>Organ</v>
+      </c>
+      <c r="O24" s="17" t="str">
+        <f>VLOOKUP(D24,[1]!VolumeType[#All],3,FALSE)</f>
+        <v>Organ</v>
+      </c>
+      <c r="P24" s="16" t="str">
+        <f>VLOOKUP(D24,[1]!Colors[#All],3,FALSE)</f>
+        <v>z Brain Stem</v>
+      </c>
+      <c r="Q24" s="14" t="str">
+        <f>IFERROR(VLOOKUP(D24,[1]!DVH_lines[#Data],2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="R24" s="15" t="str">
+        <f>IFERROR(VLOOKUP(D24,[1]!DVH_lines[#Data],3,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="S24" s="13" t="str">
+        <f>IFERROR(VLOOKUP(D24,[1]!DVH_lines[#Data],4,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="T24" s="14" t="str">
+        <f>IFERROR(VLOOKUP(D24,[1]!SearchCT[#Data],2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="U24" s="13" t="str">
+        <f>IFERROR(VLOOKUP(D24,[1]!SearchCT[#Data],3,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="25" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B25"/>
+      <c r="D25" s="72" t="s">
+        <v>257</v>
+      </c>
+      <c r="E25" s="73" t="s">
+        <v>258</v>
+      </c>
+      <c r="F25" s="74" t="s">
+        <v>259</v>
+      </c>
+      <c r="G25" s="75" t="str">
+        <f>IF(EXACT(D25,"DPV"),VLOOKUP(REPLACE($B$8,1,1,""),[1]!ICD_Codes[#All],2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="H25" s="76" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J25" s="10" t="str">
+        <f>VLOOKUP(D25,[1]!Dictionary[#All],3,FALSE)</f>
+        <v>PRV</v>
+      </c>
+      <c r="K25" s="9" t="str">
+        <f>VLOOKUP(D25,[1]!Dictionary[#All],4,FALSE)</f>
+        <v>PRV</v>
+      </c>
+      <c r="L25" s="9" t="str">
+        <f>VLOOKUP(D25,[1]!Dictionary[#All],5,FALSE)</f>
+        <v>99VMS_STRUCTCODE</v>
+      </c>
+      <c r="M25" s="8" t="str">
+        <f>VLOOKUP(D25,[1]!Dictionary[#All],6,FALSE)</f>
+        <v>1.0</v>
+      </c>
+      <c r="N25" s="7" t="str">
+        <f>VLOOKUP(D25,[1]!VolumeType[#All],2,FALSE)</f>
+        <v>Control</v>
+      </c>
+      <c r="O25" s="6" t="str">
+        <f>VLOOKUP(D25,[1]!VolumeType[#All],3,FALSE)</f>
+        <v>Avoidance</v>
+      </c>
+      <c r="P25" s="47" t="str">
+        <f>VLOOKUP(D25,[1]!Colors[#All],3,FALSE)</f>
+        <v>z BR STM PRV</v>
+      </c>
+      <c r="Q25" s="3" t="str">
+        <f>IFERROR(VLOOKUP(D25,[1]!DVH_lines[#Data],2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="R25" s="4" t="str">
+        <f>IFERROR(VLOOKUP(D25,[1]!DVH_lines[#Data],3,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="S25" s="2" t="str">
+        <f>IFERROR(VLOOKUP(D25,[1]!DVH_lines[#Data],4,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="T25" s="3" t="str">
+        <f>IFERROR(VLOOKUP(D25,[1]!SearchCT[#Data],2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="U25" s="2" t="str">
+        <f>IFERROR(VLOOKUP(D25,[1]!SearchCT[#Data],3,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:H1"/>
+    <mergeCell ref="J1:M1"/>
+    <mergeCell ref="N1:O1"/>
+    <mergeCell ref="Q1:S1"/>
+    <mergeCell ref="T1:U1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="93" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <tableParts count="2">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>